<commit_message>
Cahnged version and corrected error in mapping table
</commit_message>
<xml_diff>
--- a/docs/assets/Mapning-XDIS91-CareCommunication.xlsx
+++ b/docs/assets/Mapning-XDIS91-CareCommunication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medcomdk.sharepoint.com/sites/FHIRCareCommunication/Delte dokumenter/General/Mapningskomponent/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medcomdk-my.sharepoint.com/personal/rch_medcom_dk/Documents/RCH/CareCommunication/Konverteringsløsning/Filer til upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4356" documentId="11_50D221D0CC18943FC97F43A43C539CF23B73FCBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38379AE6-7A93-4EEE-8144-858C048090B9}"/>
+  <xr:revisionPtr revIDLastSave="4360" documentId="11_50D221D0CC18943FC97F43A43C539CF23B73FCBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA795EDA-1DCC-4286-BC6D-8C50890EFE7E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="770" firstSheet="2" activeTab="3" xr2:uid="{51F46B4B-F1EE-4E35-81E4-1D9BBBC1F172}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="770" firstSheet="1" activeTab="1" xr2:uid="{51F46B4B-F1EE-4E35-81E4-1D9BBBC1F172}"/>
   </bookViews>
   <sheets>
     <sheet name="XDIS91 -&gt; CareCommunication" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="319">
   <si>
     <t>Name</t>
   </si>
@@ -1013,12 +1013,15 @@
   <si>
     <t xml:space="preserve">Ved besvarelse og videresendelse inkluderes dette i en tekststreng. </t>
   </si>
+  <si>
+    <t>&lt;br/&gt; erstattes med &lt;Break/&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1590,17 +1593,17 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2309,9 +2312,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 Tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2349,7 +2352,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2455,7 +2458,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2597,7 +2600,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2607,21 +2610,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268600A4-E78C-42A9-8BF4-3FD7F0A9067F}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView topLeftCell="B54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="55.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="46.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30.75">
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
@@ -2659,7 +2662,7 @@
       </c>
       <c r="F2" s="44"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
@@ -2677,7 +2680,7 @@
       </c>
       <c r="F3" s="44"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="30.75">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>12</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>16</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30.75">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
         <v>20</v>
       </c>
@@ -2735,7 +2738,7 @@
       </c>
       <c r="F6" s="44"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>22</v>
       </c>
@@ -2753,7 +2756,7 @@
       </c>
       <c r="F7" s="46"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
         <v>24</v>
       </c>
@@ -2771,7 +2774,7 @@
       </c>
       <c r="F8" s="46"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
         <v>26</v>
       </c>
@@ -2789,7 +2792,7 @@
       </c>
       <c r="F9" s="46"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="43" t="s">
         <v>28</v>
       </c>
@@ -2807,7 +2810,7 @@
       </c>
       <c r="F10" s="44"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="45.75">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="100" t="s">
         <v>31</v>
       </c>
@@ -2828,7 +2831,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="45.75">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="43" t="s">
         <v>34</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
         <v>37</v>
       </c>
@@ -2866,7 +2869,7 @@
       </c>
       <c r="F13" s="46"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
         <v>39</v>
       </c>
@@ -2884,7 +2887,7 @@
       </c>
       <c r="F14" s="44"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>42</v>
       </c>
@@ -2902,7 +2905,7 @@
       </c>
       <c r="F15" s="44"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>43</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30.75">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="43" t="s">
         <v>47</v>
       </c>
@@ -2940,7 +2943,7 @@
       </c>
       <c r="F17" s="44"/>
     </row>
-    <row r="18" spans="1:6" ht="30.75">
+    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
         <v>50</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30.75">
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>54</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30.75">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>58</v>
       </c>
@@ -3000,7 +3003,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>62</v>
       </c>
@@ -3018,7 +3021,7 @@
       </c>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>64</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30.75">
+    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>66</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30.75">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>69</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>73</v>
       </c>
@@ -3096,7 +3099,7 @@
       </c>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>75</v>
       </c>
@@ -3114,7 +3117,7 @@
       </c>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>77</v>
       </c>
@@ -3132,7 +3135,7 @@
       </c>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>79</v>
       </c>
@@ -3150,7 +3153,7 @@
       </c>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>81</v>
       </c>
@@ -3168,7 +3171,7 @@
       </c>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" ht="30.75">
+    <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>83</v>
       </c>
@@ -3186,7 +3189,7 @@
       </c>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="60.75">
+    <row r="31" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>85</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30.75">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>89</v>
       </c>
@@ -3224,7 +3227,7 @@
       </c>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="30.75">
+    <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="43" t="s">
         <v>91</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30.75">
+    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
         <v>93</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="43" t="s">
         <v>96</v>
       </c>
@@ -3282,7 +3285,7 @@
       </c>
       <c r="F35" s="44"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="43" t="s">
         <v>64</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="30.75">
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="43" t="s">
         <v>98</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="30.75">
+    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="43" t="s">
         <v>99</v>
       </c>
@@ -3340,7 +3343,7 @@
       </c>
       <c r="F38" s="44"/>
     </row>
-    <row r="39" spans="1:6" ht="30.75">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="43" t="s">
         <v>101</v>
       </c>
@@ -3358,7 +3361,7 @@
       </c>
       <c r="F39" s="44"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="43" t="s">
         <v>103</v>
       </c>
@@ -3376,7 +3379,7 @@
       </c>
       <c r="F40" s="44"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="43" t="s">
         <v>105</v>
       </c>
@@ -3394,7 +3397,7 @@
       </c>
       <c r="F41" s="44"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="43" t="s">
         <v>107</v>
       </c>
@@ -3412,7 +3415,7 @@
       </c>
       <c r="F42" s="46"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="43" t="s">
         <v>109</v>
       </c>
@@ -3430,7 +3433,7 @@
       </c>
       <c r="F43" s="44"/>
     </row>
-    <row r="44" spans="1:6" ht="30.75">
+    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="43" t="s">
         <v>111</v>
       </c>
@@ -3448,7 +3451,7 @@
       </c>
       <c r="F44" s="44"/>
     </row>
-    <row r="45" spans="1:6" ht="30.75">
+    <row r="45" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>113</v>
       </c>
@@ -3468,7 +3471,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="45.75">
+    <row r="46" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>118</v>
       </c>
@@ -3486,7 +3489,7 @@
       </c>
       <c r="F46" s="7"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>121</v>
       </c>
@@ -3504,7 +3507,7 @@
       </c>
       <c r="F47" s="7"/>
     </row>
-    <row r="48" spans="1:6" ht="30.75">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>124</v>
       </c>
@@ -3522,7 +3525,7 @@
       </c>
       <c r="F48" s="7"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>127</v>
       </c>
@@ -3540,7 +3543,7 @@
       </c>
       <c r="F49" s="7"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>130</v>
       </c>
@@ -3558,7 +3561,7 @@
       </c>
       <c r="F50" s="7"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>132</v>
       </c>
@@ -3576,7 +3579,7 @@
       </c>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:6" s="52" customFormat="1" ht="30.75">
+    <row r="52" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>135</v>
       </c>
@@ -3594,7 +3597,7 @@
       </c>
       <c r="F52" s="7"/>
     </row>
-    <row r="53" spans="1:6" s="52" customFormat="1">
+    <row r="53" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>138</v>
       </c>
@@ -3612,7 +3615,7 @@
       </c>
       <c r="F53" s="7"/>
     </row>
-    <row r="54" spans="1:6" s="52" customFormat="1" ht="45.75">
+    <row r="54" spans="1:6" s="52" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="43" t="s">
         <v>140</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="52" customFormat="1" ht="30.75">
+    <row r="55" spans="1:6" s="52" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="43" t="s">
         <v>144</v>
       </c>
@@ -3652,7 +3655,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>147</v>
       </c>
@@ -3672,7 +3675,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>150</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="45.75">
+    <row r="58" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>153</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30.75">
+    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>157</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30.75">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>161</v>
       </c>
@@ -3752,7 +3755,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="351">
+    <row r="61" spans="1:6" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>165</v>
       </c>
@@ -3772,7 +3775,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>168</v>
       </c>
@@ -3792,7 +3795,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>171</v>
       </c>
@@ -3812,7 +3815,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="45.75">
+    <row r="64" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A64" s="43" t="s">
         <v>174</v>
       </c>
@@ -3830,7 +3833,7 @@
       </c>
       <c r="F64" s="46"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="43" t="s">
         <v>175</v>
       </c>
@@ -3848,7 +3851,7 @@
       </c>
       <c r="F65" s="46"/>
     </row>
-    <row r="66" spans="1:6" ht="30.75">
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="43" t="s">
         <v>176</v>
       </c>
@@ -3866,7 +3869,7 @@
       </c>
       <c r="F66" s="44"/>
     </row>
-    <row r="67" spans="1:6" ht="30.75">
+    <row r="67" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="43" t="s">
         <v>180</v>
       </c>
@@ -3884,7 +3887,7 @@
       </c>
       <c r="F67" s="44"/>
     </row>
-    <row r="68" spans="1:6" ht="30.75">
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="43" t="s">
         <v>183</v>
       </c>
@@ -3902,7 +3905,7 @@
       </c>
       <c r="F68" s="44"/>
     </row>
-    <row r="69" spans="1:6" ht="30.75">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="43" t="s">
         <v>186</v>
       </c>
@@ -3920,7 +3923,7 @@
       </c>
       <c r="F69" s="44"/>
     </row>
-    <row r="70" spans="1:6" ht="45.75">
+    <row r="70" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="43" t="s">
         <v>188</v>
       </c>
@@ -3940,7 +3943,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="30.75">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="43" t="s">
         <v>191</v>
       </c>
@@ -3958,7 +3961,7 @@
       </c>
       <c r="F71" s="46"/>
     </row>
-    <row r="72" spans="1:6" ht="30.75">
+    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="43" t="s">
         <v>193</v>
       </c>
@@ -3976,7 +3979,7 @@
       </c>
       <c r="F72" s="46"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="43" t="s">
         <v>194</v>
       </c>
@@ -3994,7 +3997,7 @@
       </c>
       <c r="F73" s="46"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>195</v>
       </c>
@@ -4012,7 +4015,7 @@
       </c>
       <c r="F74" s="7"/>
     </row>
-    <row r="75" spans="1:6" ht="30.75">
+    <row r="75" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>195</v>
       </c>
@@ -4030,7 +4033,7 @@
       </c>
       <c r="F75" s="7"/>
     </row>
-    <row r="76" spans="1:6" ht="30.75">
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>199</v>
       </c>
@@ -4050,7 +4053,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="30.75">
+    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>202</v>
       </c>
@@ -4070,7 +4073,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="30.75">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>205</v>
       </c>
@@ -4088,7 +4091,7 @@
       </c>
       <c r="F78" s="7"/>
     </row>
-    <row r="79" spans="1:6" ht="30.75">
+    <row r="79" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A79" s="43" t="s">
         <v>206</v>
       </c>
@@ -4106,7 +4109,7 @@
       </c>
       <c r="F79" s="44"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="10"/>
       <c r="C80" s="42"/>
@@ -4127,26 +4130,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A4A08-747B-4578-8C14-3B0FA19DF1A5}">
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="45.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="47.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="45.26953125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="27.26953125" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30.75">
+    <row r="1" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4175,7 +4178,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13" ht="30.75">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
@@ -4200,7 +4203,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="30.75">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
@@ -4225,7 +4228,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>16</v>
       </c>
@@ -4252,7 +4255,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>12</v>
       </c>
@@ -4277,7 +4280,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
         <v>34</v>
       </c>
@@ -4304,7 +4307,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>37</v>
       </c>
@@ -4331,7 +4334,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="30.75">
+    <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
         <v>20</v>
       </c>
@@ -4358,7 +4361,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
@@ -4383,7 +4386,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>213</v>
       </c>
@@ -4410,7 +4413,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -4435,7 +4438,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -4460,7 +4463,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
@@ -4485,7 +4488,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="97" t="s">
         <v>215</v>
       </c>
@@ -4507,10 +4510,10 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
       <c r="K14" s="31"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="115"/>
-    </row>
-    <row r="15" spans="1:13" ht="30.75">
+      <c r="L14" s="116"/>
+      <c r="M14" s="116"/>
+    </row>
+    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>216</v>
       </c>
@@ -4532,10 +4535,10 @@
       <c r="I15" s="28"/>
       <c r="J15" s="29"/>
       <c r="K15" s="28"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
-    </row>
-    <row r="16" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L15" s="116"/>
+      <c r="M15" s="116"/>
+    </row>
+    <row r="16" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>66</v>
       </c>
@@ -4557,10 +4560,10 @@
       <c r="I16" s="33"/>
       <c r="J16" s="34"/>
       <c r="K16" s="33"/>
-      <c r="L16" s="115"/>
-      <c r="M16" s="115"/>
-    </row>
-    <row r="17" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L16" s="116"/>
+      <c r="M16" s="116"/>
+    </row>
+    <row r="17" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="43" t="s">
         <v>69</v>
       </c>
@@ -4582,10 +4585,10 @@
       <c r="I17" s="33"/>
       <c r="J17" s="34"/>
       <c r="K17" s="33"/>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
-    </row>
-    <row r="18" spans="1:13" ht="117.75" customHeight="1">
+      <c r="L17" s="116"/>
+      <c r="M17" s="116"/>
+    </row>
+    <row r="18" spans="1:13" ht="117.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
         <v>58</v>
       </c>
@@ -4607,10 +4610,10 @@
       <c r="I18" s="33"/>
       <c r="J18" s="34"/>
       <c r="K18" s="33"/>
-      <c r="L18" s="115"/>
-      <c r="M18" s="115"/>
-    </row>
-    <row r="19" spans="1:13" ht="135" customHeight="1">
+      <c r="L18" s="116"/>
+      <c r="M18" s="116"/>
+    </row>
+    <row r="19" spans="1:13" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>62</v>
       </c>
@@ -4634,10 +4637,10 @@
       <c r="I19" s="109"/>
       <c r="J19" s="29"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="115"/>
-      <c r="M19" s="115"/>
-    </row>
-    <row r="20" spans="1:13" ht="30.75">
+      <c r="L19" s="116"/>
+      <c r="M19" s="116"/>
+    </row>
+    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>218</v>
       </c>
@@ -4659,10 +4662,10 @@
       <c r="I20" s="28"/>
       <c r="J20" s="29"/>
       <c r="K20" s="28"/>
-      <c r="L20" s="115"/>
-      <c r="M20" s="115"/>
-    </row>
-    <row r="21" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L20" s="116"/>
+      <c r="M20" s="116"/>
+    </row>
+    <row r="21" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>98</v>
       </c>
@@ -4684,10 +4687,10 @@
       <c r="I21" s="33"/>
       <c r="J21" s="34"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="115"/>
-      <c r="M21" s="115"/>
-    </row>
-    <row r="22" spans="1:13" ht="53.25" customHeight="1">
+      <c r="L21" s="116"/>
+      <c r="M21" s="116"/>
+    </row>
+    <row r="22" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>99</v>
       </c>
@@ -4709,10 +4712,10 @@
       <c r="I22" s="33"/>
       <c r="J22" s="34"/>
       <c r="K22" s="33"/>
-      <c r="L22" s="115"/>
-      <c r="M22" s="115"/>
-    </row>
-    <row r="23" spans="1:13" ht="55.5" customHeight="1">
+      <c r="L22" s="116"/>
+      <c r="M22" s="116"/>
+    </row>
+    <row r="23" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>93</v>
       </c>
@@ -4736,10 +4739,10 @@
       <c r="I23" s="33"/>
       <c r="J23" s="34"/>
       <c r="K23" s="33"/>
-      <c r="L23" s="115"/>
-      <c r="M23" s="115"/>
-    </row>
-    <row r="24" spans="1:13" ht="76.5">
+      <c r="L23" s="116"/>
+      <c r="M23" s="116"/>
+    </row>
+    <row r="24" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>96</v>
       </c>
@@ -4763,10 +4766,10 @@
       <c r="I24" s="31"/>
       <c r="J24" s="29"/>
       <c r="K24" s="31"/>
-      <c r="L24" s="115"/>
-      <c r="M24" s="115"/>
-    </row>
-    <row r="25" spans="1:13" ht="30.75">
+      <c r="L24" s="116"/>
+      <c r="M24" s="116"/>
+    </row>
+    <row r="25" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="43" t="s">
         <v>113</v>
       </c>
@@ -4790,10 +4793,10 @@
       <c r="I25" s="31"/>
       <c r="J25" s="29"/>
       <c r="K25" s="31"/>
-      <c r="L25" s="115"/>
-      <c r="M25" s="115"/>
-    </row>
-    <row r="26" spans="1:13" ht="45.75">
+      <c r="L25" s="116"/>
+      <c r="M25" s="116"/>
+    </row>
+    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="43" t="s">
         <v>118</v>
       </c>
@@ -4818,7 +4821,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" ht="30.75">
+    <row r="27" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="43" t="s">
         <v>121</v>
       </c>
@@ -4843,7 +4846,7 @@
       <c r="L27" s="117"/>
       <c r="M27" s="117"/>
     </row>
-    <row r="28" spans="1:13" ht="30.75">
+    <row r="28" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="43" t="s">
         <v>124</v>
       </c>
@@ -4868,7 +4871,7 @@
       <c r="L28" s="117"/>
       <c r="M28" s="117"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="43" t="s">
         <v>127</v>
       </c>
@@ -4893,7 +4896,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" ht="27.95" customHeight="1">
+    <row r="30" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="43" t="s">
         <v>132</v>
       </c>
@@ -4915,10 +4918,10 @@
       <c r="I30" s="33"/>
       <c r="J30" s="34"/>
       <c r="K30" s="33"/>
-      <c r="L30" s="115"/>
-      <c r="M30" s="115"/>
-    </row>
-    <row r="31" spans="1:13" ht="30.75">
+      <c r="L30" s="116"/>
+      <c r="M30" s="116"/>
+    </row>
+    <row r="31" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="43" t="s">
         <v>135</v>
       </c>
@@ -4939,10 +4942,10 @@
       <c r="I31" s="33"/>
       <c r="J31" s="34"/>
       <c r="K31" s="33"/>
-      <c r="L31" s="115"/>
-      <c r="M31" s="115"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="L31" s="116"/>
+      <c r="M31" s="116"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="43" t="s">
         <v>221</v>
       </c>
@@ -4966,10 +4969,10 @@
       <c r="I32" s="33"/>
       <c r="J32" s="34"/>
       <c r="K32" s="33"/>
-      <c r="L32" s="115"/>
-      <c r="M32" s="115"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="L32" s="116"/>
+      <c r="M32" s="116"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="43" t="s">
         <v>224</v>
       </c>
@@ -4991,10 +4994,10 @@
       <c r="I33" s="33"/>
       <c r="J33" s="34"/>
       <c r="K33" s="33"/>
-      <c r="L33" s="115"/>
-      <c r="M33" s="115"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="L33" s="116"/>
+      <c r="M33" s="116"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
         <v>224</v>
       </c>
@@ -5016,10 +5019,10 @@
       <c r="I34" s="33"/>
       <c r="J34" s="34"/>
       <c r="K34" s="33"/>
-      <c r="L34" s="115"/>
-      <c r="M34" s="115"/>
-    </row>
-    <row r="35" spans="1:13" ht="30.75">
+      <c r="L34" s="116"/>
+      <c r="M34" s="116"/>
+    </row>
+    <row r="35" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>50</v>
       </c>
@@ -5043,10 +5046,10 @@
       <c r="I35" s="33"/>
       <c r="J35" s="34"/>
       <c r="K35" s="33"/>
-      <c r="L35" s="115"/>
-      <c r="M35" s="115"/>
-    </row>
-    <row r="36" spans="1:13" ht="45.75">
+      <c r="L35" s="116"/>
+      <c r="M35" s="116"/>
+    </row>
+    <row r="36" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>140</v>
       </c>
@@ -5070,10 +5073,10 @@
       <c r="I36" s="33"/>
       <c r="J36" s="34"/>
       <c r="K36" s="33"/>
-      <c r="L36" s="115"/>
-      <c r="M36" s="115"/>
-    </row>
-    <row r="37" spans="1:13" ht="30.75">
+      <c r="L36" s="116"/>
+      <c r="M36" s="116"/>
+    </row>
+    <row r="37" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="105" t="s">
         <v>144</v>
       </c>
@@ -5095,10 +5098,10 @@
       <c r="I37" s="33"/>
       <c r="J37" s="34"/>
       <c r="K37" s="33"/>
-      <c r="L37" s="115"/>
-      <c r="M37" s="115"/>
-    </row>
-    <row r="38" spans="1:13" ht="30.75">
+      <c r="L37" s="116"/>
+      <c r="M37" s="116"/>
+    </row>
+    <row r="38" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="43" t="s">
         <v>147</v>
       </c>
@@ -5122,10 +5125,10 @@
       <c r="I38" s="33"/>
       <c r="J38" s="34"/>
       <c r="K38" s="33"/>
-      <c r="L38" s="115"/>
-      <c r="M38" s="115"/>
-    </row>
-    <row r="39" spans="1:13" ht="60.75">
+      <c r="L38" s="116"/>
+      <c r="M38" s="116"/>
+    </row>
+    <row r="39" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="43" t="s">
         <v>150</v>
       </c>
@@ -5149,10 +5152,10 @@
       <c r="I39" s="33"/>
       <c r="J39" s="34"/>
       <c r="K39" s="33"/>
-      <c r="L39" s="115"/>
-      <c r="M39" s="115"/>
-    </row>
-    <row r="40" spans="1:13" ht="30.75">
+      <c r="L39" s="116"/>
+      <c r="M39" s="116"/>
+    </row>
+    <row r="40" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="43" t="s">
         <v>153</v>
       </c>
@@ -5176,10 +5179,10 @@
       <c r="I40" s="33"/>
       <c r="J40" s="34"/>
       <c r="K40" s="33"/>
-      <c r="L40" s="115"/>
-      <c r="M40" s="115"/>
-    </row>
-    <row r="41" spans="1:13" ht="30.75">
+      <c r="L40" s="116"/>
+      <c r="M40" s="116"/>
+    </row>
+    <row r="41" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="43" t="s">
         <v>157</v>
       </c>
@@ -5201,10 +5204,10 @@
       <c r="I41" s="33"/>
       <c r="J41" s="34"/>
       <c r="K41" s="33"/>
-      <c r="L41" s="115"/>
-      <c r="M41" s="115"/>
-    </row>
-    <row r="42" spans="1:13" ht="30.75">
+      <c r="L41" s="116"/>
+      <c r="M41" s="116"/>
+    </row>
+    <row r="42" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>161</v>
       </c>
@@ -5220,18 +5223,18 @@
       <c r="E42" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="9" t="s">
-        <v>164</v>
+      <c r="F42" s="7" t="s">
+        <v>318</v>
       </c>
       <c r="G42" s="113"/>
       <c r="H42" s="34"/>
       <c r="I42" s="33"/>
       <c r="J42" s="34"/>
       <c r="K42" s="33"/>
-      <c r="L42" s="115"/>
-      <c r="M42" s="115"/>
-    </row>
-    <row r="43" spans="1:13" ht="30.75">
+      <c r="L42" s="116"/>
+      <c r="M42" s="116"/>
+    </row>
+    <row r="43" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>39</v>
       </c>
@@ -5253,10 +5256,10 @@
       <c r="I43" s="31"/>
       <c r="J43" s="29"/>
       <c r="K43" s="31"/>
-      <c r="L43" s="115"/>
-      <c r="M43" s="115"/>
-    </row>
-    <row r="44" spans="1:13" ht="30.75">
+      <c r="L43" s="116"/>
+      <c r="M43" s="116"/>
+    </row>
+    <row r="44" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>42</v>
       </c>
@@ -5278,10 +5281,10 @@
       <c r="I44" s="31"/>
       <c r="J44" s="29"/>
       <c r="K44" s="31"/>
-      <c r="L44" s="115"/>
-      <c r="M44" s="115"/>
-    </row>
-    <row r="45" spans="1:13" ht="30.75">
+      <c r="L44" s="116"/>
+      <c r="M44" s="116"/>
+    </row>
+    <row r="45" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>168</v>
       </c>
@@ -5305,10 +5308,10 @@
       <c r="I45" s="31"/>
       <c r="J45" s="29"/>
       <c r="K45" s="31"/>
-      <c r="L45" s="115"/>
-      <c r="M45" s="115"/>
-    </row>
-    <row r="46" spans="1:13" ht="30.75">
+      <c r="L45" s="116"/>
+      <c r="M45" s="116"/>
+    </row>
+    <row r="46" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>171</v>
       </c>
@@ -5332,10 +5335,10 @@
       <c r="I46" s="31"/>
       <c r="J46" s="29"/>
       <c r="K46" s="31"/>
-      <c r="L46" s="115"/>
-      <c r="M46" s="115"/>
-    </row>
-    <row r="47" spans="1:13" ht="30.75">
+      <c r="L46" s="116"/>
+      <c r="M46" s="116"/>
+    </row>
+    <row r="47" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>232</v>
       </c>
@@ -5360,7 +5363,7 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:13" ht="30.75">
+    <row r="48" spans="1:13" ht="31.5" x14ac:dyDescent="0.6">
       <c r="A48" s="43" t="s">
         <v>176</v>
       </c>
@@ -5387,7 +5390,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="30.75">
+    <row r="49" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="43" t="s">
         <v>180</v>
       </c>
@@ -5409,10 +5412,10 @@
       <c r="I49" s="36"/>
       <c r="J49" s="20"/>
       <c r="K49" s="36"/>
-      <c r="L49" s="116"/>
-      <c r="M49" s="116"/>
-    </row>
-    <row r="50" spans="1:13" ht="30.75">
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+    </row>
+    <row r="50" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="43" t="s">
         <v>183</v>
       </c>
@@ -5436,10 +5439,10 @@
       <c r="I50" s="36"/>
       <c r="J50" s="20"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="116"/>
-      <c r="M50" s="116"/>
-    </row>
-    <row r="51" spans="1:13" ht="30.75">
+      <c r="L50" s="118"/>
+      <c r="M50" s="118"/>
+    </row>
+    <row r="51" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="43" t="s">
         <v>188</v>
       </c>
@@ -5466,7 +5469,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
     </row>
-    <row r="52" spans="1:13" ht="30.75">
+    <row r="52" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="43" t="s">
         <v>191</v>
       </c>
@@ -5488,10 +5491,10 @@
       <c r="I52" s="32"/>
       <c r="J52" s="22"/>
       <c r="K52" s="32"/>
-      <c r="L52" s="115"/>
-      <c r="M52" s="115"/>
-    </row>
-    <row r="53" spans="1:13" ht="30.75">
+      <c r="L52" s="116"/>
+      <c r="M52" s="116"/>
+    </row>
+    <row r="53" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="43" t="s">
         <v>237</v>
       </c>
@@ -5513,10 +5516,10 @@
       <c r="I53" s="33"/>
       <c r="J53" s="34"/>
       <c r="K53" s="33"/>
-      <c r="L53" s="115"/>
-      <c r="M53" s="115"/>
-    </row>
-    <row r="54" spans="1:13" ht="30.75">
+      <c r="L53" s="116"/>
+      <c r="M53" s="116"/>
+    </row>
+    <row r="54" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="43" t="s">
         <v>238</v>
       </c>
@@ -5538,10 +5541,10 @@
       <c r="I54" s="33"/>
       <c r="J54" s="34"/>
       <c r="K54" s="33"/>
-      <c r="L54" s="115"/>
-      <c r="M54" s="115"/>
-    </row>
-    <row r="55" spans="1:13" ht="30.75">
+      <c r="L54" s="116"/>
+      <c r="M54" s="116"/>
+    </row>
+    <row r="55" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="43" t="s">
         <v>239</v>
       </c>
@@ -5563,10 +5566,10 @@
       <c r="I55" s="33"/>
       <c r="J55" s="34"/>
       <c r="K55" s="33"/>
-      <c r="L55" s="115"/>
-      <c r="M55" s="115"/>
-    </row>
-    <row r="56" spans="1:13" ht="30.75">
+      <c r="L55" s="116"/>
+      <c r="M55" s="116"/>
+    </row>
+    <row r="56" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="43" t="s">
         <v>241</v>
       </c>
@@ -5588,10 +5591,10 @@
       <c r="I56" s="33"/>
       <c r="J56" s="34"/>
       <c r="K56" s="33"/>
-      <c r="L56" s="115"/>
-      <c r="M56" s="115"/>
-    </row>
-    <row r="57" spans="1:13" ht="30.75">
+      <c r="L56" s="116"/>
+      <c r="M56" s="116"/>
+    </row>
+    <row r="57" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="43" t="s">
         <v>186</v>
       </c>
@@ -5615,10 +5618,10 @@
       <c r="I57" s="33"/>
       <c r="J57" s="34"/>
       <c r="K57" s="33"/>
-      <c r="L57" s="115"/>
-      <c r="M57" s="115"/>
-    </row>
-    <row r="58" spans="1:13" ht="30.75">
+      <c r="L57" s="116"/>
+      <c r="M57" s="116"/>
+    </row>
+    <row r="58" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>199</v>
       </c>
@@ -5640,10 +5643,10 @@
       <c r="I58" s="33"/>
       <c r="J58" s="34"/>
       <c r="K58" s="33"/>
-      <c r="L58" s="115"/>
-      <c r="M58" s="115"/>
-    </row>
-    <row r="59" spans="1:13" ht="30.75">
+      <c r="L58" s="116"/>
+      <c r="M58" s="116"/>
+    </row>
+    <row r="59" spans="1:13" ht="31" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="9" t="s">
         <v>202</v>
       </c>
@@ -5668,7 +5671,7 @@
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:13" ht="30.75">
+    <row r="60" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>243</v>
       </c>
@@ -5693,7 +5696,7 @@
       <c r="L60" s="6"/>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="1:13" ht="30.75">
+    <row r="61" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>205</v>
       </c>
@@ -5718,7 +5721,7 @@
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>245</v>
       </c>
@@ -5743,7 +5746,7 @@
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
     </row>
-    <row r="63" spans="1:13" ht="23.25">
+    <row r="63" spans="1:13" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>246</v>
       </c>
@@ -5768,7 +5771,7 @@
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
     </row>
-    <row r="64" spans="1:13" ht="30.75">
+    <row r="64" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>247</v>
       </c>
@@ -5793,7 +5796,7 @@
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
     </row>
-    <row r="65" spans="1:13" ht="45.75">
+    <row r="65" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A65" s="43" t="s">
         <v>248</v>
       </c>
@@ -5820,7 +5823,7 @@
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
     </row>
-    <row r="66" spans="1:13" ht="45.75">
+    <row r="66" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A66" s="43" t="s">
         <v>250</v>
       </c>
@@ -5847,7 +5850,7 @@
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
     </row>
-    <row r="67" spans="1:13" ht="30.75">
+    <row r="67" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>206</v>
       </c>
@@ -5872,7 +5875,7 @@
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
     </row>
-    <row r="68" spans="1:13" ht="30.75">
+    <row r="68" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>47</v>
       </c>
@@ -5896,10 +5899,10 @@
       <c r="I68" s="31"/>
       <c r="J68" s="29"/>
       <c r="K68" s="28"/>
-      <c r="L68" s="116"/>
-      <c r="M68" s="116"/>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="L68" s="118"/>
+      <c r="M68" s="118"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>252</v>
       </c>
@@ -5923,10 +5926,10 @@
       <c r="I69" s="31"/>
       <c r="J69" s="29"/>
       <c r="K69" s="28"/>
-      <c r="L69" s="116"/>
-      <c r="M69" s="116"/>
-    </row>
-    <row r="70" spans="1:13" ht="45.75">
+      <c r="L69" s="118"/>
+      <c r="M69" s="118"/>
+    </row>
+    <row r="70" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>255</v>
       </c>
@@ -5950,10 +5953,10 @@
       <c r="I70" s="31"/>
       <c r="J70" s="29"/>
       <c r="K70" s="28"/>
-      <c r="L70" s="116"/>
-      <c r="M70" s="116"/>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="L70" s="118"/>
+      <c r="M70" s="118"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>215</v>
       </c>
@@ -5978,7 +5981,7 @@
       <c r="L71" s="6"/>
       <c r="M71" s="6"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="7"/>
       <c r="C72" s="11"/>
@@ -5993,7 +5996,7 @@
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="7"/>
       <c r="C73" s="11"/>
@@ -6005,10 +6008,10 @@
       <c r="I73" s="31"/>
       <c r="J73" s="29"/>
       <c r="K73" s="28"/>
-      <c r="L73" s="116"/>
-      <c r="M73" s="116"/>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="L73" s="118"/>
+      <c r="M73" s="118"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="7"/>
       <c r="C74" s="11"/>
@@ -6020,10 +6023,10 @@
       <c r="I74" s="31"/>
       <c r="J74" s="29"/>
       <c r="K74" s="28"/>
-      <c r="L74" s="116"/>
-      <c r="M74" s="116"/>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="L74" s="118"/>
+      <c r="M74" s="118"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F75" s="30"/>
       <c r="G75" s="28"/>
       <c r="H75" s="29"/>
@@ -6033,7 +6036,7 @@
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F76" s="27"/>
       <c r="G76" s="28"/>
       <c r="H76" s="29"/>
@@ -6043,7 +6046,7 @@
       <c r="L76" s="37"/>
       <c r="M76" s="37"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F77" s="27"/>
       <c r="G77" s="19"/>
       <c r="H77" s="20"/>
@@ -6053,7 +6056,7 @@
       <c r="L77" s="6"/>
       <c r="M77" s="6"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F78" s="27"/>
       <c r="G78" s="19"/>
       <c r="H78" s="20"/>
@@ -6063,7 +6066,7 @@
       <c r="L78" s="6"/>
       <c r="M78" s="6"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="F79" s="30"/>
       <c r="G79" s="19"/>
       <c r="H79" s="20"/>
@@ -6073,7 +6076,7 @@
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="1:13" ht="26.25">
+    <row r="80" spans="1:13" ht="26" x14ac:dyDescent="0.6">
       <c r="F80" s="27"/>
       <c r="G80" s="26"/>
       <c r="H80" s="17"/>
@@ -6083,7 +6086,7 @@
       <c r="L80" s="6"/>
       <c r="M80" s="6"/>
     </row>
-    <row r="81" spans="6:13">
+    <row r="81" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F81" s="27"/>
       <c r="G81" s="28"/>
       <c r="H81" s="29"/>
@@ -6093,7 +6096,7 @@
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="82" spans="6:13">
+    <row r="82" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F82" s="27"/>
       <c r="G82" s="28"/>
       <c r="H82" s="29"/>
@@ -6103,7 +6106,7 @@
       <c r="L82" s="6"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="6:13">
+    <row r="83" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F83" s="27"/>
       <c r="G83" s="28"/>
       <c r="H83" s="29"/>
@@ -6113,7 +6116,7 @@
       <c r="L83" s="6"/>
       <c r="M83" s="6"/>
     </row>
-    <row r="84" spans="6:13">
+    <row r="84" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F84" s="27"/>
       <c r="G84" s="28"/>
       <c r="H84" s="29"/>
@@ -6123,32 +6126,44 @@
       <c r="L84" s="6"/>
       <c r="M84" s="6"/>
     </row>
-    <row r="85" spans="6:13">
+    <row r="85" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F85" s="18"/>
     </row>
-    <row r="86" spans="6:13">
+    <row r="86" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F86" s="18"/>
     </row>
-    <row r="87" spans="6:13">
+    <row r="87" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="6:13">
+    <row r="88" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F88" s="25"/>
     </row>
-    <row r="89" spans="6:13">
+    <row r="89" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F89" s="27"/>
     </row>
-    <row r="90" spans="6:13">
+    <row r="90" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F90" s="27"/>
     </row>
-    <row r="91" spans="6:13">
+    <row r="91" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F91" s="27"/>
     </row>
-    <row r="92" spans="6:13">
+    <row r="92" spans="6:13" x14ac:dyDescent="0.35">
       <c r="F92" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L52:L58"/>
+    <mergeCell ref="M52:M58"/>
+    <mergeCell ref="L68:L70"/>
+    <mergeCell ref="M68:M70"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="M49:M50"/>
     <mergeCell ref="L30:L32"/>
     <mergeCell ref="M30:M32"/>
     <mergeCell ref="L33:L42"/>
@@ -6157,18 +6172,6 @@
     <mergeCell ref="M14:M25"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="M49:M50"/>
-    <mergeCell ref="L52:L58"/>
-    <mergeCell ref="M52:M58"/>
-    <mergeCell ref="L68:L70"/>
-    <mergeCell ref="M68:M70"/>
-    <mergeCell ref="L73:L74"/>
-    <mergeCell ref="M73:M74"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6183,23 +6186,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7BD392-D2FE-48CB-ABD4-43BFAD774472}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="D54" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30.75">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
@@ -6253,7 +6256,7 @@
       <c r="H2" s="44"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9" ht="30.75">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
@@ -6278,7 +6281,7 @@
       <c r="H3" s="44"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="30.75">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>12</v>
       </c>
@@ -6305,7 +6308,7 @@
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>16</v>
       </c>
@@ -6332,7 +6335,7 @@
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="30.75">
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
         <v>20</v>
       </c>
@@ -6357,7 +6360,7 @@
       <c r="H6" s="44"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>22</v>
       </c>
@@ -6382,7 +6385,7 @@
       <c r="H7" s="46"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="30.75">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
         <v>24</v>
       </c>
@@ -6407,7 +6410,7 @@
       <c r="H8" s="46"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
         <v>26</v>
       </c>
@@ -6432,7 +6435,7 @@
       <c r="H9" s="46"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="30.75">
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="43" t="s">
         <v>28</v>
       </c>
@@ -6457,7 +6460,7 @@
       <c r="H10" s="44"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="60.75">
+    <row r="11" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="100" t="s">
         <v>215</v>
       </c>
@@ -6484,7 +6487,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="30.75">
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="43" t="s">
         <v>34</v>
       </c>
@@ -6509,7 +6512,7 @@
       <c r="H12" s="44"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="30.75">
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
         <v>37</v>
       </c>
@@ -6534,7 +6537,7 @@
       <c r="H13" s="46"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="30.75">
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="43" t="s">
         <v>39</v>
       </c>
@@ -6559,7 +6562,7 @@
       <c r="H14" s="44"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>42</v>
       </c>
@@ -6584,7 +6587,7 @@
       <c r="H15" s="44"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="30.75">
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>43</v>
       </c>
@@ -6611,7 +6614,7 @@
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" ht="30.75">
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43" t="s">
         <v>47</v>
       </c>
@@ -6636,7 +6639,7 @@
       <c r="H17" s="44"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" ht="30.75">
+    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
         <v>50</v>
       </c>
@@ -6663,7 +6666,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="30.75">
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>54</v>
       </c>
@@ -6690,7 +6693,7 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="30.75">
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>58</v>
       </c>
@@ -6717,7 +6720,7 @@
       </c>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="30.75">
+    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>62</v>
       </c>
@@ -6742,7 +6745,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="30.75">
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>66</v>
       </c>
@@ -6769,7 +6772,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="30.75">
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>69</v>
       </c>
@@ -6796,7 +6799,7 @@
       </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="30.75">
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>73</v>
       </c>
@@ -6821,7 +6824,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="30.75">
+    <row r="25" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>75</v>
       </c>
@@ -6846,7 +6849,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="30.75">
+    <row r="26" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>77</v>
       </c>
@@ -6871,7 +6874,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="30.75">
+    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>79</v>
       </c>
@@ -6896,7 +6899,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="30.75">
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>81</v>
       </c>
@@ -6921,7 +6924,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="30.75">
+    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>83</v>
       </c>
@@ -6946,7 +6949,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="76.5">
+    <row r="30" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>85</v>
       </c>
@@ -6973,7 +6976,7 @@
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="30.75">
+    <row r="31" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>89</v>
       </c>
@@ -6998,7 +7001,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="30.75">
+    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="43" t="s">
         <v>91</v>
       </c>
@@ -7025,7 +7028,7 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="30.75">
+    <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="43" t="s">
         <v>93</v>
       </c>
@@ -7052,7 +7055,7 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="30.75">
+    <row r="34" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
         <v>96</v>
       </c>
@@ -7077,7 +7080,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="30.75">
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="43" t="s">
         <v>98</v>
       </c>
@@ -7104,7 +7107,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="30.75">
+    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="43" t="s">
         <v>99</v>
       </c>
@@ -7129,7 +7132,7 @@
       <c r="H36" s="44"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="30.75">
+    <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="43" t="s">
         <v>101</v>
       </c>
@@ -7154,7 +7157,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="30.75">
+    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="43" t="s">
         <v>103</v>
       </c>
@@ -7179,7 +7182,7 @@
       <c r="H38" s="44"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="30.75">
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="43" t="s">
         <v>105</v>
       </c>
@@ -7204,7 +7207,7 @@
       <c r="H39" s="44"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="30.75">
+    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="43" t="s">
         <v>107</v>
       </c>
@@ -7229,7 +7232,7 @@
       <c r="H40" s="46"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="30.75">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="43" t="s">
         <v>109</v>
       </c>
@@ -7254,7 +7257,7 @@
       <c r="H41" s="44"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" ht="30.75">
+    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="43" t="s">
         <v>111</v>
       </c>
@@ -7279,7 +7282,7 @@
       <c r="H42" s="44"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:9" ht="45.75">
+    <row r="43" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>113</v>
       </c>
@@ -7306,7 +7309,7 @@
       </c>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:9" ht="45.75">
+    <row r="44" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>118</v>
       </c>
@@ -7333,7 +7336,7 @@
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" ht="30.75">
+    <row r="45" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>121</v>
       </c>
@@ -7358,7 +7361,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:9" ht="30.75">
+    <row r="46" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>124</v>
       </c>
@@ -7383,7 +7386,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="1:9" ht="30.75">
+    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>127</v>
       </c>
@@ -7408,7 +7411,7 @@
       <c r="H47" s="7"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="1:9" ht="30.75">
+    <row r="48" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>130</v>
       </c>
@@ -7433,7 +7436,7 @@
       <c r="H48" s="7"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="1:9" ht="30.75">
+    <row r="49" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>132</v>
       </c>
@@ -7458,7 +7461,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="1:9" ht="30.75">
+    <row r="50" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>135</v>
       </c>
@@ -7483,7 +7486,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="1:9" ht="30.75">
+    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>138</v>
       </c>
@@ -7508,7 +7511,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="1:9" ht="30.75">
+    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>17</v>
       </c>
@@ -7535,7 +7538,7 @@
       </c>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="1:9" ht="30.75">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>17</v>
       </c>
@@ -7562,7 +7565,7 @@
       </c>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="1:9" ht="45.75">
+    <row r="54" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="43" t="s">
         <v>140</v>
       </c>
@@ -7589,7 +7592,7 @@
       </c>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="1:9" ht="30.75">
+    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="108" t="s">
         <v>144</v>
       </c>
@@ -7616,7 +7619,7 @@
       </c>
       <c r="I55" s="10"/>
     </row>
-    <row r="56" spans="1:9" ht="30.75">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>147</v>
       </c>
@@ -7643,7 +7646,7 @@
       </c>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>150</v>
       </c>
@@ -7670,7 +7673,7 @@
       </c>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="1:9" ht="45.75">
+    <row r="58" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>153</v>
       </c>
@@ -7697,7 +7700,7 @@
       </c>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="1:9" ht="30.75">
+    <row r="59" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>157</v>
       </c>
@@ -7724,7 +7727,7 @@
       </c>
       <c r="I59" s="10"/>
     </row>
-    <row r="60" spans="1:9" ht="30.75">
+    <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>161</v>
       </c>
@@ -7751,7 +7754,7 @@
       </c>
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="1:9" ht="409.6">
+    <row r="61" spans="1:9" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>165</v>
       </c>
@@ -7770,7 +7773,7 @@
       </c>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" spans="1:9" ht="409.6">
+    <row r="62" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>302</v>
       </c>
@@ -7797,7 +7800,7 @@
       </c>
       <c r="I62" s="10"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>168</v>
       </c>
@@ -7824,7 +7827,7 @@
       </c>
       <c r="I63" s="10"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>171</v>
       </c>
@@ -7851,7 +7854,7 @@
       </c>
       <c r="I64" s="10"/>
     </row>
-    <row r="65" spans="1:9" ht="30.75">
+    <row r="65" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="43" t="s">
         <v>176</v>
       </c>
@@ -7876,7 +7879,7 @@
       <c r="H65" s="44"/>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="1:9" ht="30.75">
+    <row r="66" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="43" t="s">
         <v>180</v>
       </c>
@@ -7901,7 +7904,7 @@
       <c r="H66" s="44"/>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" spans="1:9" ht="30.75">
+    <row r="67" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="43" t="s">
         <v>183</v>
       </c>
@@ -7926,7 +7929,7 @@
       <c r="H67" s="44"/>
       <c r="I67" s="10"/>
     </row>
-    <row r="68" spans="1:9" ht="30.75">
+    <row r="68" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="43" t="s">
         <v>186</v>
       </c>
@@ -7951,7 +7954,7 @@
       <c r="H68" s="44"/>
       <c r="I68" s="10"/>
     </row>
-    <row r="69" spans="1:9" ht="30.75">
+    <row r="69" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="43" t="s">
         <v>188</v>
       </c>
@@ -7976,7 +7979,7 @@
       <c r="H69" s="46"/>
       <c r="I69" s="10"/>
     </row>
-    <row r="70" spans="1:9" ht="30.75">
+    <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="43" t="s">
         <v>191</v>
       </c>
@@ -8001,7 +8004,7 @@
       <c r="H70" s="46"/>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="1:9" ht="30.75">
+    <row r="71" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>195</v>
       </c>
@@ -8026,7 +8029,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="1:9" ht="30.75">
+    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>195</v>
       </c>
@@ -8051,7 +8054,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="10"/>
     </row>
-    <row r="73" spans="1:9" ht="30.75">
+    <row r="73" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>199</v>
       </c>
@@ -8078,7 +8081,7 @@
       </c>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9" ht="30.75">
+    <row r="74" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>202</v>
       </c>
@@ -8105,7 +8108,7 @@
       </c>
       <c r="I74" s="10"/>
     </row>
-    <row r="75" spans="1:9" ht="30.75">
+    <row r="75" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>205</v>
       </c>
@@ -8130,7 +8133,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="10"/>
     </row>
-    <row r="76" spans="1:9" ht="30.75">
+    <row r="76" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A76" s="43" t="s">
         <v>206</v>
       </c>
@@ -8155,7 +8158,7 @@
       <c r="H76" s="44"/>
       <c r="I76" s="10"/>
     </row>
-    <row r="77" spans="1:9" ht="60.75">
+    <row r="77" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>215</v>
       </c>
@@ -8195,23 +8198,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018E8C56-7845-49A6-99BD-BE444F662575}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="82" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="83" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="82" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="37.453125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" style="82" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="83" customWidth="1"/>
+    <col min="6" max="6" width="44.7265625" style="82" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" customWidth="1"/>
+    <col min="8" max="8" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -8238,7 +8241,7 @@
       </c>
       <c r="I1" s="72"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
@@ -8263,7 +8266,7 @@
       <c r="H2" s="44"/>
       <c r="I2" s="72"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>10</v>
       </c>
@@ -8287,7 +8290,7 @@
       </c>
       <c r="H3" s="44"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>16</v>
       </c>
@@ -8312,7 +8315,7 @@
       </c>
       <c r="I4" s="73"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>12</v>
       </c>
@@ -8336,7 +8339,7 @@
       </c>
       <c r="H5" s="44"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
         <v>34</v>
       </c>
@@ -8363,7 +8366,7 @@
       </c>
       <c r="I6" s="73"/>
     </row>
-    <row r="7" spans="1:9" ht="30.75">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>37</v>
       </c>
@@ -8390,7 +8393,7 @@
       </c>
       <c r="I7" s="73"/>
     </row>
-    <row r="8" spans="1:9" ht="30.75">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
         <v>20</v>
       </c>
@@ -8417,7 +8420,7 @@
       </c>
       <c r="I8" s="73"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
@@ -8441,7 +8444,7 @@
       </c>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>213</v>
       </c>
@@ -8467,7 +8470,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30.75">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
@@ -8491,7 +8494,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="30.75">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -8515,7 +8518,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>26</v>
       </c>
@@ -8539,7 +8542,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="97" t="s">
         <v>215</v>
       </c>
@@ -8563,7 +8566,7 @@
       </c>
       <c r="H14" s="99"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="43" t="s">
         <v>216</v>
       </c>
@@ -8587,7 +8590,7 @@
       </c>
       <c r="H15" s="44"/>
     </row>
-    <row r="16" spans="1:9" ht="30.75">
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>66</v>
       </c>
@@ -8612,7 +8615,7 @@
       <c r="H16" s="44"/>
       <c r="I16" s="73"/>
     </row>
-    <row r="17" spans="1:9" ht="30.75">
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="43" t="s">
         <v>69</v>
       </c>
@@ -8636,7 +8639,7 @@
       </c>
       <c r="H17" s="44"/>
     </row>
-    <row r="18" spans="1:9" ht="30.75">
+    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="43" t="s">
         <v>58</v>
       </c>
@@ -8660,7 +8663,7 @@
       </c>
       <c r="H18" s="111"/>
     </row>
-    <row r="19" spans="1:9" ht="30.75">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
         <v>62</v>
       </c>
@@ -8686,7 +8689,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30.75">
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>218</v>
       </c>
@@ -8711,7 +8714,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="73"/>
     </row>
-    <row r="21" spans="1:9" ht="30.75">
+    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>98</v>
       </c>
@@ -8735,7 +8738,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="30.75">
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>99</v>
       </c>
@@ -8760,7 +8763,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="73"/>
     </row>
-    <row r="23" spans="1:9" ht="45.75">
+    <row r="23" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>93</v>
       </c>
@@ -8787,7 +8790,7 @@
       </c>
       <c r="I23" s="73"/>
     </row>
-    <row r="24" spans="1:9" ht="106.5">
+    <row r="24" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>96</v>
       </c>
@@ -8814,7 +8817,7 @@
       </c>
       <c r="I24" s="73"/>
     </row>
-    <row r="25" spans="1:9" ht="30.75">
+    <row r="25" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="43" t="s">
         <v>113</v>
       </c>
@@ -8841,7 +8844,7 @@
       </c>
       <c r="I25" s="73"/>
     </row>
-    <row r="26" spans="1:9" ht="45.75">
+    <row r="26" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="43" t="s">
         <v>118</v>
       </c>
@@ -8868,7 +8871,7 @@
       </c>
       <c r="I26" s="73"/>
     </row>
-    <row r="27" spans="1:9" ht="30.75">
+    <row r="27" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="43" t="s">
         <v>121</v>
       </c>
@@ -8893,7 +8896,7 @@
       <c r="H27" s="44"/>
       <c r="I27" s="73"/>
     </row>
-    <row r="28" spans="1:9" ht="30.75">
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="43" t="s">
         <v>124</v>
       </c>
@@ -8918,7 +8921,7 @@
       <c r="H28" s="44"/>
       <c r="I28" s="73"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="43" t="s">
         <v>127</v>
       </c>
@@ -8943,7 +8946,7 @@
       <c r="H29" s="44"/>
       <c r="I29" s="73"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="43" t="s">
         <v>132</v>
       </c>
@@ -8967,7 +8970,7 @@
       </c>
       <c r="H30" s="44"/>
     </row>
-    <row r="31" spans="1:9" ht="30.75">
+    <row r="31" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="43" t="s">
         <v>135</v>
       </c>
@@ -8991,7 +8994,7 @@
       </c>
       <c r="H31" s="44"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="43" t="s">
         <v>221</v>
       </c>
@@ -9017,7 +9020,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="43" t="s">
         <v>224</v>
       </c>
@@ -9042,7 +9045,7 @@
       <c r="H33" s="46"/>
       <c r="I33" s="73"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="43" t="s">
         <v>224</v>
       </c>
@@ -9067,7 +9070,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="73"/>
     </row>
-    <row r="35" spans="1:9" ht="30.75">
+    <row r="35" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>50</v>
       </c>
@@ -9094,7 +9097,7 @@
       </c>
       <c r="I35" s="73"/>
     </row>
-    <row r="36" spans="1:9" ht="45.75">
+    <row r="36" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>140</v>
       </c>
@@ -9121,7 +9124,7 @@
       </c>
       <c r="I36" s="73"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="105" t="s">
         <v>144</v>
       </c>
@@ -9146,7 +9149,7 @@
       <c r="H37" s="107"/>
       <c r="I37" s="73"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="43" t="s">
         <v>147</v>
       </c>
@@ -9173,7 +9176,7 @@
       </c>
       <c r="I38" s="73"/>
     </row>
-    <row r="39" spans="1:9" ht="60.75">
+    <row r="39" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="43" t="s">
         <v>150</v>
       </c>
@@ -9200,7 +9203,7 @@
       </c>
       <c r="I39" s="73"/>
     </row>
-    <row r="40" spans="1:9" ht="30.75">
+    <row r="40" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="43" t="s">
         <v>153</v>
       </c>
@@ -9227,7 +9230,7 @@
       </c>
       <c r="I40" s="73"/>
     </row>
-    <row r="41" spans="1:9" ht="30.75">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="43" t="s">
         <v>157</v>
       </c>
@@ -9252,7 +9255,7 @@
       <c r="H41" s="43"/>
       <c r="I41" s="73"/>
     </row>
-    <row r="42" spans="1:9" ht="30.75">
+    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>161</v>
       </c>
@@ -9275,10 +9278,10 @@
         <v>17</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="30.75">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>39</v>
       </c>
@@ -9302,7 +9305,7 @@
       </c>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:9" ht="30.75">
+    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>42</v>
       </c>
@@ -9326,7 +9329,7 @@
       </c>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:9" ht="30.75">
+    <row r="45" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>168</v>
       </c>
@@ -9352,7 +9355,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30.75">
+    <row r="46" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>171</v>
       </c>
@@ -9379,7 +9382,7 @@
       </c>
       <c r="I46" s="73"/>
     </row>
-    <row r="47" spans="1:9" ht="30.75">
+    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>232</v>
       </c>
@@ -9404,7 +9407,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="73"/>
     </row>
-    <row r="48" spans="1:9" ht="45.75">
+    <row r="48" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="43" t="s">
         <v>176</v>
       </c>
@@ -9426,12 +9429,12 @@
       <c r="G48" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="118" t="s">
+      <c r="H48" s="115" t="s">
         <v>314</v>
       </c>
       <c r="I48" s="73"/>
     </row>
-    <row r="49" spans="1:9" ht="30.75">
+    <row r="49" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="43" t="s">
         <v>180</v>
       </c>
@@ -9456,7 +9459,7 @@
       <c r="H49" s="44"/>
       <c r="I49" s="73"/>
     </row>
-    <row r="50" spans="1:9" ht="30.75">
+    <row r="50" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="43" t="s">
         <v>183</v>
       </c>
@@ -9483,7 +9486,7 @@
       </c>
       <c r="I50" s="73"/>
     </row>
-    <row r="51" spans="1:9" ht="30.75">
+    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="43" t="s">
         <v>188</v>
       </c>
@@ -9510,7 +9513,7 @@
       </c>
       <c r="I51" s="73"/>
     </row>
-    <row r="52" spans="1:9" ht="30.75">
+    <row r="52" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="43" t="s">
         <v>191</v>
       </c>
@@ -9535,7 +9538,7 @@
       <c r="H52" s="44"/>
       <c r="I52" s="73"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="43" t="s">
         <v>237</v>
       </c>
@@ -9560,7 +9563,7 @@
       <c r="H53" s="44"/>
       <c r="I53" s="73"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="43" t="s">
         <v>238</v>
       </c>
@@ -9585,7 +9588,7 @@
       <c r="H54" s="44"/>
       <c r="I54" s="73"/>
     </row>
-    <row r="55" spans="1:9" ht="30.75">
+    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="43" t="s">
         <v>239</v>
       </c>
@@ -9610,7 +9613,7 @@
       <c r="H55" s="46"/>
       <c r="I55" s="73"/>
     </row>
-    <row r="56" spans="1:9" ht="30.75">
+    <row r="56" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="43" t="s">
         <v>241</v>
       </c>
@@ -9635,7 +9638,7 @@
       <c r="H56" s="44"/>
       <c r="I56" s="73"/>
     </row>
-    <row r="57" spans="1:9" ht="30.75">
+    <row r="57" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="43" t="s">
         <v>186</v>
       </c>
@@ -9661,7 +9664,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30.75">
+    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>199</v>
       </c>
@@ -9685,7 +9688,7 @@
       </c>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="1:9" ht="30.75">
+    <row r="59" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>202</v>
       </c>
@@ -9709,7 +9712,7 @@
       </c>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="30.75">
+    <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>243</v>
       </c>
@@ -9733,7 +9736,7 @@
       </c>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="1:9" ht="30.75">
+    <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>205</v>
       </c>
@@ -9758,7 +9761,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="73"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>245</v>
       </c>
@@ -9783,7 +9786,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="75"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>246</v>
       </c>
@@ -9808,7 +9811,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="75"/>
     </row>
-    <row r="64" spans="1:9" ht="30.75">
+    <row r="64" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>247</v>
       </c>
@@ -9833,7 +9836,7 @@
       <c r="H64" s="10"/>
       <c r="I64" s="75"/>
     </row>
-    <row r="65" spans="1:9" ht="60.75">
+    <row r="65" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" s="43" t="s">
         <v>248</v>
       </c>
@@ -9860,7 +9863,7 @@
       </c>
       <c r="I65" s="73"/>
     </row>
-    <row r="66" spans="1:9" ht="60.75">
+    <row r="66" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" s="43" t="s">
         <v>315</v>
       </c>
@@ -9887,7 +9890,7 @@
       </c>
       <c r="I66" s="74"/>
     </row>
-    <row r="67" spans="1:9" ht="30.75">
+    <row r="67" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>206</v>
       </c>
@@ -9912,7 +9915,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="74"/>
     </row>
-    <row r="68" spans="1:9" ht="30.75">
+    <row r="68" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>47</v>
       </c>
@@ -9939,7 +9942,7 @@
       </c>
       <c r="I68" s="74"/>
     </row>
-    <row r="69" spans="1:9" ht="30.75">
+    <row r="69" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>252</v>
       </c>
@@ -9965,7 +9968,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="60.75">
+    <row r="70" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>255</v>
       </c>
@@ -9991,7 +9994,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="63"/>
       <c r="C71" s="11"/>
@@ -10001,7 +10004,7 @@
       <c r="G71" s="54"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="63"/>
       <c r="C72" s="11"/>
@@ -10011,7 +10014,7 @@
       <c r="G72" s="54"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="63"/>
       <c r="C73" s="11"/>
@@ -10021,7 +10024,7 @@
       <c r="G73" s="11"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="63"/>
       <c r="C74" s="11"/>
@@ -10041,6 +10044,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CE3A8153F207434E9AE9E016B63FAED4" ma:contentTypeVersion="8" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="7f40f411f573b8fe8b54b03a91a915e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee8ef5dc-6422-4132-ba28-a9150fefde4c" xmlns:ns3="672a50b0-1df9-4341-9d54-48b9c706e195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f743c63ff20ddb338bfd710406406b29" ns2:_="" ns3:_="">
     <xsd:import namespace="ee8ef5dc-6422-4132-ba28-a9150fefde4c"/>
@@ -10229,12 +10238,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10245,13 +10248,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F52A3E-A96F-430E-A3B0-81F6F960E42E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E44D686-25A5-46EE-BE4F-34D7EEAF48C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E44D686-25A5-46EE-BE4F-34D7EEAF48C5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5F52A3E-A96F-430E-A3B0-81F6F960E42E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee8ef5dc-6422-4132-ba28-a9150fefde4c"/>
+    <ds:schemaRef ds:uri="672a50b0-1df9-4341-9d54-48b9c706e195"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912B5AAF-FD1D-4092-AB11-BCD9ECA30C35}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912B5AAF-FD1D-4092-AB11-BCD9ECA30C35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated test examples and mapping table
</commit_message>
<xml_diff>
--- a/docs/assets/Mapning-XDIS91-CareCommunication.xlsx
+++ b/docs/assets/Mapning-XDIS91-CareCommunication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28724"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://medcomdk.sharepoint.com/sites/FHIRCareCommunication/Delte dokumenter/General/Konverteringsløsning/Mapningskomponent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B05407BB-628F-42F0-B960-A8E05B865A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4454" documentId="11_50D221D0CC18943FC97F43A43C539CF23B73FCBC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E74390C-6D64-4E88-9F92-2B670D9FC12B}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="770" firstSheet="3" activeTab="1" xr2:uid="{51F46B4B-F1EE-4E35-81E4-1D9BBBC1F172}"/>
+    <workbookView xWindow="19090" yWindow="-600" windowWidth="19420" windowHeight="11500" tabRatio="770" activeTab="2" xr2:uid="{51F46B4B-F1EE-4E35-81E4-1D9BBBC1F172}"/>
   </bookViews>
   <sheets>
     <sheet name="XDIS91 -&gt; CareCommunication" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="326">
   <si>
     <t>Name</t>
   </si>
@@ -721,9 +721,6 @@
 Hvis systemet er Ydernummer: indsæt 'ydernummer'.</t>
   </si>
   <si>
-    <t>Patient.identifier.where(system = ‘https://sundhedsdatastyrelsen.dk/da/registre-og-services/ecpr’).value</t>
-  </si>
-  <si>
     <t>Deceased</t>
   </si>
   <si>
@@ -816,9 +813,6 @@
   </si>
   <si>
     <t>Specific recipient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ved besvarelse, videresendelse, rettelse og annullering inkluderes dette i en tekststreng. </t>
   </si>
   <si>
     <t>Previous message</t>
@@ -1026,14 +1020,31 @@
     <t>Emessage.ClinicalEmail.ClinicalInformation.Text02</t>
   </si>
   <si>
-    <t xml:space="preserve">Ved besvarelse og videresendelse inkluderes dette i en tekststreng. </t>
+    <t>Default: new-message i CareCommunication</t>
+  </si>
+  <si>
+    <t>Ved besvarelse og videresendelse, inkluderes dette i Text01</t>
+  </si>
+  <si>
+    <t>Patient.identifier.where(system = 'xxx’**).value</t>
+  </si>
+  <si>
+    <t>* Det er mandatory at sende medsende en identifier, enten CPR eller erstatnings-CPR.
+**Systemet 'xxx' i CareCommunication er baseret på følgende: Hvis position nr. 7 i erstatnings-CPR har tallet '1' eller '7' bruges system: urn:oid:1.2.208.176.1.6.1.1. Ellers bruges system: urn:oid:1.2.208.176.1.6.1.3.</t>
+  </si>
+  <si>
+    <t>* Det er mandatory at sende medsende en identifier, enten CPR eller erstatnings-CPR.
+**Systemet 'xxx' i CareCommunication er baseret på følgende: Hvis position nr. 7 i erstatnings-CPR har tallet '1' eller '7' bruges system: urn:oid:1.2.208.176.1.6.1.1. Ellers bruges system: urn:oid:1.2.208.176.1.6.1.3.</t>
+  </si>
+  <si>
+    <t>Patient.identifier.where(system = ‘xxx’**).value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1292,7 +1303,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1632,35 +1643,41 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2401,9 +2418,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 Tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2441,7 +2458,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2547,7 +2564,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2689,7 +2706,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2699,11 +2716,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{268600A4-E78C-42A9-8BF4-3FD7F0A9067F}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
@@ -2714,7 +2731,7 @@
     <col min="7" max="7" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.1">
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>7</v>
       </c>
@@ -2756,7 +2773,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>11</v>
       </c>
@@ -2775,7 +2792,7 @@
       <c r="F3" s="44"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="29.1">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>13</v>
       </c>
@@ -2796,7 +2813,7 @@
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1">
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>17</v>
       </c>
@@ -2817,7 +2834,7 @@
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>21</v>
       </c>
@@ -2836,7 +2853,7 @@
       <c r="F6" s="44"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>23</v>
       </c>
@@ -2855,7 +2872,7 @@
       <c r="F7" s="46"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>25</v>
       </c>
@@ -2874,7 +2891,7 @@
       <c r="F8" s="46"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
         <v>27</v>
       </c>
@@ -2893,7 +2910,7 @@
       <c r="F9" s="46"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
         <v>29</v>
       </c>
@@ -2912,7 +2929,7 @@
       <c r="F10" s="44"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="43.5">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="96" t="s">
         <v>32</v>
       </c>
@@ -2933,7 +2950,7 @@
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="43.5">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>35</v>
       </c>
@@ -2954,7 +2971,7 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>38</v>
       </c>
@@ -2973,7 +2990,7 @@
       <c r="F13" s="46"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
         <v>40</v>
       </c>
@@ -2992,7 +3009,7 @@
       <c r="F14" s="44"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>43</v>
       </c>
@@ -3011,7 +3028,7 @@
       <c r="F15" s="44"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>45</v>
       </c>
@@ -3032,7 +3049,7 @@
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>49</v>
       </c>
@@ -3048,10 +3065,12 @@
       <c r="E17" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="44"/>
+      <c r="F17" s="126" t="s">
+        <v>320</v>
+      </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" ht="29.1">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>52</v>
       </c>
@@ -3072,7 +3091,7 @@
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" ht="30.75">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
@@ -3082,7 +3101,7 @@
       <c r="C19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="120" t="s">
         <v>58</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -3093,7 +3112,7 @@
       </c>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>60</v>
       </c>
@@ -3114,7 +3133,7 @@
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>64</v>
       </c>
@@ -3133,7 +3152,7 @@
       <c r="F21" s="8"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>66</v>
       </c>
@@ -3154,7 +3173,7 @@
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" ht="29.1">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>68</v>
       </c>
@@ -3175,7 +3194,7 @@
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" ht="29.1">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>71</v>
       </c>
@@ -3196,7 +3215,7 @@
       </c>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>75</v>
       </c>
@@ -3215,7 +3234,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>77</v>
       </c>
@@ -3234,7 +3253,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>79</v>
       </c>
@@ -3253,7 +3272,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>81</v>
       </c>
@@ -3272,7 +3291,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>83</v>
       </c>
@@ -3291,7 +3310,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" ht="29.1">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>85</v>
       </c>
@@ -3310,7 +3329,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" ht="57.95">
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>87</v>
       </c>
@@ -3331,7 +3350,7 @@
       </c>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>91</v>
       </c>
@@ -3350,7 +3369,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" ht="30.75">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
         <v>93</v>
       </c>
@@ -3360,7 +3379,7 @@
       <c r="C33" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="120" t="s">
+      <c r="D33" s="117" t="s">
         <v>58</v>
       </c>
       <c r="E33" s="45" t="s">
@@ -3371,7 +3390,7 @@
       </c>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:7" ht="29.1">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
         <v>95</v>
       </c>
@@ -3392,7 +3411,7 @@
       </c>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
         <v>98</v>
       </c>
@@ -3411,7 +3430,7 @@
       <c r="F35" s="44"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
         <v>66</v>
       </c>
@@ -3432,7 +3451,7 @@
       </c>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:7" ht="29.1">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>100</v>
       </c>
@@ -3453,7 +3472,7 @@
       </c>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:7" ht="29.1">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
         <v>101</v>
       </c>
@@ -3472,7 +3491,7 @@
       <c r="F38" s="44"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>103</v>
       </c>
@@ -3491,7 +3510,7 @@
       <c r="F39" s="44"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>105</v>
       </c>
@@ -3510,7 +3529,7 @@
       <c r="F40" s="44"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>107</v>
       </c>
@@ -3529,7 +3548,7 @@
       <c r="F41" s="44"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
         <v>109</v>
       </c>
@@ -3548,7 +3567,7 @@
       <c r="F42" s="46"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
         <v>111</v>
       </c>
@@ -3567,7 +3586,7 @@
       <c r="F43" s="44"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" ht="29.1">
+    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
         <v>113</v>
       </c>
@@ -3586,7 +3605,7 @@
       <c r="F44" s="44"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" ht="29.1">
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>115</v>
       </c>
@@ -3607,7 +3626,7 @@
       </c>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:7" ht="43.5">
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>120</v>
       </c>
@@ -3628,7 +3647,7 @@
       </c>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>124</v>
       </c>
@@ -3647,7 +3666,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>127</v>
       </c>
@@ -3666,7 +3685,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="10"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>130</v>
       </c>
@@ -3685,7 +3704,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>133</v>
       </c>
@@ -3704,7 +3723,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>135</v>
       </c>
@@ -3723,7 +3742,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:7" s="52" customFormat="1">
+    <row r="52" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>138</v>
       </c>
@@ -3742,7 +3761,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:7" s="52" customFormat="1">
+    <row r="53" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>141</v>
       </c>
@@ -3761,7 +3780,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="1:7" s="52" customFormat="1" ht="43.5">
+    <row r="54" spans="1:7" s="52" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="43" t="s">
         <v>143</v>
       </c>
@@ -3782,7 +3801,7 @@
       </c>
       <c r="G54" s="10"/>
     </row>
-    <row r="55" spans="1:7" s="52" customFormat="1" ht="29.1">
+    <row r="55" spans="1:7" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
         <v>147</v>
       </c>
@@ -3803,7 +3822,7 @@
       </c>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>150</v>
       </c>
@@ -3824,7 +3843,7 @@
       </c>
       <c r="G56" s="10"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>153</v>
       </c>
@@ -3845,7 +3864,7 @@
       </c>
       <c r="G57" s="10"/>
     </row>
-    <row r="58" spans="1:7" ht="76.5">
+    <row r="58" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>156</v>
       </c>
@@ -3861,12 +3880,12 @@
       <c r="E58" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F58" s="125" t="s">
+      <c r="F58" s="121" t="s">
         <v>159</v>
       </c>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="1:7" ht="29.1">
+    <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>160</v>
       </c>
@@ -3887,7 +3906,7 @@
       </c>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" spans="1:7" ht="72.599999999999994">
+    <row r="60" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>164</v>
       </c>
@@ -3908,7 +3927,7 @@
       </c>
       <c r="G60" s="112"/>
     </row>
-    <row r="61" spans="1:7" ht="333.6">
+    <row r="61" spans="1:7" ht="360" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>168</v>
       </c>
@@ -3929,7 +3948,7 @@
       </c>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>171</v>
       </c>
@@ -3950,7 +3969,7 @@
       </c>
       <c r="G62" s="10"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>174</v>
       </c>
@@ -3971,7 +3990,7 @@
       </c>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" spans="1:7" ht="43.5">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="43" t="s">
         <v>177</v>
       </c>
@@ -3990,7 +4009,7 @@
       <c r="F64" s="46"/>
       <c r="G64" s="10"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>178</v>
       </c>
@@ -4009,7 +4028,7 @@
       <c r="F65" s="46"/>
       <c r="G65" s="10"/>
     </row>
-    <row r="66" spans="1:7" ht="29.1">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>179</v>
       </c>
@@ -4028,7 +4047,7 @@
       <c r="F66" s="44"/>
       <c r="G66" s="10"/>
     </row>
-    <row r="67" spans="1:7" ht="29.1">
+    <row r="67" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>183</v>
       </c>
@@ -4047,7 +4066,7 @@
       <c r="F67" s="44"/>
       <c r="G67" s="10"/>
     </row>
-    <row r="68" spans="1:7" ht="29.1">
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>186</v>
       </c>
@@ -4066,7 +4085,7 @@
       <c r="F68" s="44"/>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="43" t="s">
         <v>189</v>
       </c>
@@ -4085,7 +4104,7 @@
       <c r="F69" s="44"/>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" spans="1:7" ht="43.5">
+    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="43" t="s">
         <v>191</v>
       </c>
@@ -4106,7 +4125,7 @@
       </c>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
         <v>194</v>
       </c>
@@ -4125,7 +4144,7 @@
       <c r="F71" s="46"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="1:7" ht="29.1">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="43" t="s">
         <v>196</v>
       </c>
@@ -4144,7 +4163,7 @@
       <c r="F72" s="46"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="43" t="s">
         <v>197</v>
       </c>
@@ -4163,7 +4182,7 @@
       <c r="F73" s="46"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>198</v>
       </c>
@@ -4182,7 +4201,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" spans="1:7" ht="29.1">
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>198</v>
       </c>
@@ -4201,7 +4220,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="10"/>
     </row>
-    <row r="76" spans="1:7" ht="29.1">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>202</v>
       </c>
@@ -4222,7 +4241,7 @@
       </c>
       <c r="G76" s="10"/>
     </row>
-    <row r="77" spans="1:7" ht="29.1">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>205</v>
       </c>
@@ -4243,7 +4262,7 @@
       </c>
       <c r="G77" s="10"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>208</v>
       </c>
@@ -4262,7 +4281,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="10"/>
     </row>
-    <row r="79" spans="1:7" ht="29.1">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="43" t="s">
         <v>209</v>
       </c>
@@ -4281,7 +4300,7 @@
       <c r="F79" s="44"/>
       <c r="G79" s="10"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
       <c r="B80" s="10"/>
       <c r="C80" s="42"/>
@@ -4293,8 +4312,9 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4303,11 +4323,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990A4A08-747B-4578-8C14-3B0FA19DF1A5}">
   <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="1" customWidth="1"/>
@@ -4322,7 +4342,7 @@
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="29.1">
+    <row r="1" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4351,7 +4371,7 @@
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>7</v>
       </c>
@@ -4376,7 +4396,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>11</v>
       </c>
@@ -4401,7 +4421,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>17</v>
       </c>
@@ -4428,7 +4448,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>13</v>
       </c>
@@ -4453,7 +4473,7 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>35</v>
       </c>
@@ -4480,7 +4500,7 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>38</v>
       </c>
@@ -4507,7 +4527,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="29.1">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>21</v>
       </c>
@@ -4534,7 +4554,7 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -4559,7 +4579,7 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>215</v>
       </c>
@@ -4586,7 +4606,7 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
@@ -4611,7 +4631,7 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -4636,7 +4656,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
@@ -4661,7 +4681,7 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="93" t="s">
         <v>217</v>
       </c>
@@ -4683,14 +4703,14 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
       <c r="K14" s="31"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-    </row>
-    <row r="15" spans="1:13" ht="30.75">
+      <c r="L14" s="123"/>
+      <c r="M14" s="123"/>
+    </row>
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="120" t="s">
+      <c r="B15" s="117" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="45" t="s">
@@ -4708,10 +4728,10 @@
       <c r="I15" s="28"/>
       <c r="J15" s="29"/>
       <c r="K15" s="28"/>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
-    </row>
-    <row r="16" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L15" s="123"/>
+      <c r="M15" s="123"/>
+    </row>
+    <row r="16" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>68</v>
       </c>
@@ -4733,10 +4753,10 @@
       <c r="I16" s="33"/>
       <c r="J16" s="34"/>
       <c r="K16" s="33"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-    </row>
-    <row r="17" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L16" s="123"/>
+      <c r="M16" s="123"/>
+    </row>
+    <row r="17" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>71</v>
       </c>
@@ -4758,10 +4778,10 @@
       <c r="I17" s="33"/>
       <c r="J17" s="34"/>
       <c r="K17" s="33"/>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
-    </row>
-    <row r="18" spans="1:13" ht="117.75" customHeight="1">
+      <c r="L17" s="123"/>
+      <c r="M17" s="123"/>
+    </row>
+    <row r="18" spans="1:13" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>60</v>
       </c>
@@ -4783,10 +4803,10 @@
       <c r="I18" s="33"/>
       <c r="J18" s="34"/>
       <c r="K18" s="33"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-    </row>
-    <row r="19" spans="1:13" ht="135" customHeight="1">
+      <c r="L18" s="123"/>
+      <c r="M18" s="123"/>
+    </row>
+    <row r="19" spans="1:13" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>64</v>
       </c>
@@ -4810,14 +4830,14 @@
       <c r="I19" s="105"/>
       <c r="J19" s="29"/>
       <c r="K19" s="31"/>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
-    </row>
-    <row r="20" spans="1:13" ht="30.75">
+      <c r="L19" s="123"/>
+      <c r="M19" s="123"/>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="124" t="s">
+      <c r="B20" s="120" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -4835,10 +4855,10 @@
       <c r="I20" s="28"/>
       <c r="J20" s="29"/>
       <c r="K20" s="28"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
-    </row>
-    <row r="21" spans="1:13" ht="27.95" customHeight="1">
+      <c r="L20" s="123"/>
+      <c r="M20" s="123"/>
+    </row>
+    <row r="21" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>100</v>
       </c>
@@ -4860,10 +4880,10 @@
       <c r="I21" s="33"/>
       <c r="J21" s="34"/>
       <c r="K21" s="33"/>
-      <c r="L21" s="117"/>
-      <c r="M21" s="117"/>
-    </row>
-    <row r="22" spans="1:13" ht="53.25" customHeight="1">
+      <c r="L21" s="123"/>
+      <c r="M21" s="123"/>
+    </row>
+    <row r="22" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>101</v>
       </c>
@@ -4885,10 +4905,10 @@
       <c r="I22" s="33"/>
       <c r="J22" s="34"/>
       <c r="K22" s="33"/>
-      <c r="L22" s="117"/>
-      <c r="M22" s="117"/>
-    </row>
-    <row r="23" spans="1:13" ht="55.5" customHeight="1">
+      <c r="L22" s="123"/>
+      <c r="M22" s="123"/>
+    </row>
+    <row r="23" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>95</v>
       </c>
@@ -4912,10 +4932,10 @@
       <c r="I23" s="33"/>
       <c r="J23" s="34"/>
       <c r="K23" s="33"/>
-      <c r="L23" s="117"/>
-      <c r="M23" s="117"/>
-    </row>
-    <row r="24" spans="1:13" ht="72.599999999999994">
+      <c r="L23" s="123"/>
+      <c r="M23" s="123"/>
+    </row>
+    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>98</v>
       </c>
@@ -4939,10 +4959,10 @@
       <c r="I24" s="31"/>
       <c r="J24" s="29"/>
       <c r="K24" s="31"/>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
-    </row>
-    <row r="25" spans="1:13" ht="29.1">
+      <c r="L24" s="123"/>
+      <c r="M24" s="123"/>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
         <v>115</v>
       </c>
@@ -4966,15 +4986,15 @@
       <c r="I25" s="31"/>
       <c r="J25" s="29"/>
       <c r="K25" s="31"/>
-      <c r="L25" s="117"/>
-      <c r="M25" s="117"/>
-    </row>
-    <row r="26" spans="1:13" ht="43.5">
+      <c r="L25" s="123"/>
+      <c r="M25" s="123"/>
+    </row>
+    <row r="26" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="44" t="s">
-        <v>223</v>
+      <c r="B26" s="126" t="s">
+        <v>325</v>
       </c>
       <c r="C26" s="45" t="s">
         <v>117</v>
@@ -4985,7 +5005,9 @@
       <c r="E26" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="44"/>
+      <c r="F26" s="126" t="s">
+        <v>324</v>
+      </c>
       <c r="G26" s="109"/>
       <c r="H26" s="22"/>
       <c r="I26" s="32"/>
@@ -4994,7 +5016,7 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
-    <row r="27" spans="1:13" ht="29.1">
+    <row r="27" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
         <v>124</v>
       </c>
@@ -5016,10 +5038,10 @@
       <c r="I27" s="28"/>
       <c r="J27" s="29"/>
       <c r="K27" s="31"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-    </row>
-    <row r="28" spans="1:13" ht="29.1">
+      <c r="L27" s="125"/>
+      <c r="M27" s="125"/>
+    </row>
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>127</v>
       </c>
@@ -5041,10 +5063,10 @@
       <c r="I28" s="28"/>
       <c r="J28" s="29"/>
       <c r="K28" s="31"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="L28" s="125"/>
+      <c r="M28" s="125"/>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>130</v>
       </c>
@@ -5069,7 +5091,7 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
     </row>
-    <row r="30" spans="1:13" ht="27.95" customHeight="1">
+    <row r="30" spans="1:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
         <v>135</v>
       </c>
@@ -5091,10 +5113,10 @@
       <c r="I30" s="33"/>
       <c r="J30" s="34"/>
       <c r="K30" s="33"/>
-      <c r="L30" s="117"/>
-      <c r="M30" s="117"/>
-    </row>
-    <row r="31" spans="1:13" ht="29.1">
+      <c r="L30" s="123"/>
+      <c r="M30" s="123"/>
+    </row>
+    <row r="31" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
         <v>138</v>
       </c>
@@ -5115,42 +5137,42 @@
       <c r="I31" s="33"/>
       <c r="J31" s="34"/>
       <c r="K31" s="33"/>
-      <c r="L31" s="117"/>
-      <c r="M31" s="117"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="L31" s="123"/>
+      <c r="M31" s="123"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="C32" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="46" t="s">
         <v>225</v>
-      </c>
-      <c r="C32" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="46" t="s">
-        <v>226</v>
       </c>
       <c r="G32" s="110"/>
       <c r="H32"/>
       <c r="I32" s="33"/>
       <c r="J32" s="34"/>
       <c r="K32" s="33"/>
-      <c r="L32" s="117"/>
-      <c r="M32" s="117"/>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="L32" s="123"/>
+      <c r="M32" s="123"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="46" t="s">
         <v>227</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>228</v>
       </c>
       <c r="C33" s="47" t="s">
         <v>18</v>
@@ -5167,15 +5189,15 @@
       <c r="I33" s="33"/>
       <c r="J33" s="34"/>
       <c r="K33" s="33"/>
-      <c r="L33" s="117"/>
-      <c r="M33" s="117"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="L33" s="123"/>
+      <c r="M33" s="123"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" s="45" t="s">
         <v>18</v>
@@ -5192,10 +5214,10 @@
       <c r="I34" s="33"/>
       <c r="J34" s="34"/>
       <c r="K34" s="33"/>
-      <c r="L34" s="117"/>
-      <c r="M34" s="117"/>
-    </row>
-    <row r="35" spans="1:13" ht="29.1">
+      <c r="L34" s="123"/>
+      <c r="M34" s="123"/>
+    </row>
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>52</v>
       </c>
@@ -5219,10 +5241,10 @@
       <c r="I35" s="33"/>
       <c r="J35" s="34"/>
       <c r="K35" s="33"/>
-      <c r="L35" s="117"/>
-      <c r="M35" s="117"/>
-    </row>
-    <row r="36" spans="1:13" ht="43.5">
+      <c r="L35" s="123"/>
+      <c r="M35" s="123"/>
+    </row>
+    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>143</v>
       </c>
@@ -5246,10 +5268,10 @@
       <c r="I36" s="33"/>
       <c r="J36" s="34"/>
       <c r="K36" s="33"/>
-      <c r="L36" s="117"/>
-      <c r="M36" s="117"/>
-    </row>
-    <row r="37" spans="1:13" ht="29.1">
+      <c r="L36" s="123"/>
+      <c r="M36" s="123"/>
+    </row>
+    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="101" t="s">
         <v>147</v>
       </c>
@@ -5271,10 +5293,10 @@
       <c r="I37" s="33"/>
       <c r="J37" s="34"/>
       <c r="K37" s="33"/>
-      <c r="L37" s="117"/>
-      <c r="M37" s="117"/>
-    </row>
-    <row r="38" spans="1:13" ht="29.1">
+      <c r="L37" s="123"/>
+      <c r="M37" s="123"/>
+    </row>
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
         <v>150</v>
       </c>
@@ -5291,17 +5313,17 @@
         <v>18</v>
       </c>
       <c r="F38" s="46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G38" s="109"/>
       <c r="H38" s="34"/>
       <c r="I38" s="33"/>
       <c r="J38" s="34"/>
       <c r="K38" s="33"/>
-      <c r="L38" s="117"/>
-      <c r="M38" s="117"/>
-    </row>
-    <row r="39" spans="1:13" ht="43.5">
+      <c r="L38" s="123"/>
+      <c r="M38" s="123"/>
+    </row>
+    <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>153</v>
       </c>
@@ -5318,17 +5340,17 @@
         <v>18</v>
       </c>
       <c r="F39" s="46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G39" s="109"/>
       <c r="H39" s="34"/>
       <c r="I39" s="33"/>
       <c r="J39" s="34"/>
       <c r="K39" s="33"/>
-      <c r="L39" s="117"/>
-      <c r="M39" s="117"/>
-    </row>
-    <row r="40" spans="1:13" ht="30.75">
+      <c r="L39" s="123"/>
+      <c r="M39" s="123"/>
+    </row>
+    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>156</v>
       </c>
@@ -5345,17 +5367,17 @@
         <v>18</v>
       </c>
       <c r="F40" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G40" s="109"/>
       <c r="H40" s="34"/>
       <c r="I40" s="33"/>
       <c r="J40" s="34"/>
       <c r="K40" s="33"/>
-      <c r="L40" s="117"/>
-      <c r="M40" s="117"/>
-    </row>
-    <row r="41" spans="1:13" ht="29.1">
+      <c r="L40" s="123"/>
+      <c r="M40" s="123"/>
+    </row>
+    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>160</v>
       </c>
@@ -5377,10 +5399,10 @@
       <c r="I41" s="33"/>
       <c r="J41" s="34"/>
       <c r="K41" s="33"/>
-      <c r="L41" s="117"/>
-      <c r="M41" s="117"/>
-    </row>
-    <row r="42" spans="1:13" ht="72.599999999999994">
+      <c r="L41" s="123"/>
+      <c r="M41" s="123"/>
+    </row>
+    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>164</v>
       </c>
@@ -5397,22 +5419,22 @@
         <v>9</v>
       </c>
       <c r="F42" s="115" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G42" s="112"/>
       <c r="H42" s="34"/>
       <c r="I42" s="33"/>
       <c r="J42" s="34"/>
       <c r="K42" s="33"/>
-      <c r="L42" s="117"/>
-      <c r="M42" s="117"/>
-    </row>
-    <row r="43" spans="1:13" ht="29.1">
+      <c r="L42" s="123"/>
+      <c r="M42" s="123"/>
+    </row>
+    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>9</v>
@@ -5429,15 +5451,15 @@
       <c r="I43" s="31"/>
       <c r="J43" s="29"/>
       <c r="K43" s="31"/>
-      <c r="L43" s="117"/>
-      <c r="M43" s="117"/>
-    </row>
-    <row r="44" spans="1:13" ht="29.1">
+      <c r="L43" s="123"/>
+      <c r="M43" s="123"/>
+    </row>
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>9</v>
@@ -5454,10 +5476,10 @@
       <c r="I44" s="31"/>
       <c r="J44" s="29"/>
       <c r="K44" s="31"/>
-      <c r="L44" s="117"/>
-      <c r="M44" s="117"/>
-    </row>
-    <row r="45" spans="1:13" ht="29.1">
+      <c r="L44" s="123"/>
+      <c r="M44" s="123"/>
+    </row>
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>171</v>
       </c>
@@ -5474,17 +5496,17 @@
         <v>9</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G45" s="53"/>
       <c r="H45" s="29"/>
       <c r="I45" s="31"/>
       <c r="J45" s="29"/>
       <c r="K45" s="31"/>
-      <c r="L45" s="117"/>
-      <c r="M45" s="117"/>
-    </row>
-    <row r="46" spans="1:13" ht="29.1">
+      <c r="L45" s="123"/>
+      <c r="M45" s="123"/>
+    </row>
+    <row r="46" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>174</v>
       </c>
@@ -5501,22 +5523,22 @@
         <v>9</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G46" s="53"/>
       <c r="H46" s="29"/>
       <c r="I46" s="31"/>
       <c r="J46" s="29"/>
       <c r="K46" s="31"/>
-      <c r="L46" s="117"/>
-      <c r="M46" s="117"/>
-    </row>
-    <row r="47" spans="1:13" ht="29.1">
+      <c r="L46" s="123"/>
+      <c r="M46" s="123"/>
+    </row>
+    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>9</v>
@@ -5536,7 +5558,7 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
     </row>
-    <row r="48" spans="1:13" ht="31.5">
+    <row r="48" spans="1:13" ht="32.25" x14ac:dyDescent="0.4">
       <c r="A48" s="43" t="s">
         <v>179</v>
       </c>
@@ -5553,7 +5575,7 @@
         <v>181</v>
       </c>
       <c r="F48" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G48" s="53"/>
       <c r="H48" s="17"/>
@@ -5563,7 +5585,7 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="29.1">
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="43" t="s">
         <v>183</v>
       </c>
@@ -5585,10 +5607,10 @@
       <c r="I49" s="36"/>
       <c r="J49" s="20"/>
       <c r="K49" s="36"/>
-      <c r="L49" s="119"/>
-      <c r="M49" s="119"/>
-    </row>
-    <row r="50" spans="1:13" ht="29.1">
+      <c r="L49" s="124"/>
+      <c r="M49" s="124"/>
+    </row>
+    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="43" t="s">
         <v>186</v>
       </c>
@@ -5605,17 +5627,17 @@
         <v>181</v>
       </c>
       <c r="F50" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G50" s="92"/>
       <c r="H50" s="20"/>
       <c r="I50" s="36"/>
       <c r="J50" s="20"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="119"/>
-      <c r="M50" s="119"/>
-    </row>
-    <row r="51" spans="1:13" ht="29.1">
+      <c r="L50" s="124"/>
+      <c r="M50" s="124"/>
+    </row>
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="43" t="s">
         <v>191</v>
       </c>
@@ -5626,13 +5648,13 @@
         <v>181</v>
       </c>
       <c r="D51" s="46" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E51" s="50" t="s">
         <v>181</v>
       </c>
       <c r="F51" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G51" s="53"/>
       <c r="H51" s="20"/>
@@ -5642,7 +5664,7 @@
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
     </row>
-    <row r="52" spans="1:13" ht="29.1">
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="43" t="s">
         <v>194</v>
       </c>
@@ -5664,12 +5686,12 @@
       <c r="I52" s="32"/>
       <c r="J52" s="22"/>
       <c r="K52" s="32"/>
-      <c r="L52" s="117"/>
-      <c r="M52" s="117"/>
-    </row>
-    <row r="53" spans="1:13" ht="29.1">
+      <c r="L52" s="123"/>
+      <c r="M52" s="123"/>
+    </row>
+    <row r="53" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B53" s="44" t="s">
         <v>172</v>
@@ -5689,12 +5711,12 @@
       <c r="I53" s="33"/>
       <c r="J53" s="34"/>
       <c r="K53" s="33"/>
-      <c r="L53" s="117"/>
-      <c r="M53" s="117"/>
-    </row>
-    <row r="54" spans="1:13" ht="29.1">
+      <c r="L53" s="123"/>
+      <c r="M53" s="123"/>
+    </row>
+    <row r="54" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B54" s="44" t="s">
         <v>175</v>
@@ -5714,15 +5736,15 @@
       <c r="I54" s="33"/>
       <c r="J54" s="34"/>
       <c r="K54" s="33"/>
-      <c r="L54" s="117"/>
-      <c r="M54" s="117"/>
-    </row>
-    <row r="55" spans="1:13" ht="29.1">
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+    </row>
+    <row r="55" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" s="44" t="s">
         <v>243</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>244</v>
       </c>
       <c r="C55" s="45" t="s">
         <v>18</v>
@@ -5739,15 +5761,15 @@
       <c r="I55" s="33"/>
       <c r="J55" s="34"/>
       <c r="K55" s="33"/>
-      <c r="L55" s="117"/>
-      <c r="M55" s="117"/>
-    </row>
-    <row r="56" spans="1:13" ht="29.1">
+      <c r="L55" s="123"/>
+      <c r="M55" s="123"/>
+    </row>
+    <row r="56" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B56" s="44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" s="45" t="s">
         <v>18</v>
@@ -5764,10 +5786,10 @@
       <c r="I56" s="33"/>
       <c r="J56" s="34"/>
       <c r="K56" s="33"/>
-      <c r="L56" s="117"/>
-      <c r="M56" s="117"/>
-    </row>
-    <row r="57" spans="1:13" ht="29.1">
+      <c r="L56" s="123"/>
+      <c r="M56" s="123"/>
+    </row>
+    <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
         <v>189</v>
       </c>
@@ -5784,17 +5806,17 @@
         <v>181</v>
       </c>
       <c r="F57" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G57" s="109"/>
       <c r="H57" s="34"/>
       <c r="I57" s="33"/>
       <c r="J57" s="34"/>
       <c r="K57" s="33"/>
-      <c r="L57" s="117"/>
-      <c r="M57" s="117"/>
-    </row>
-    <row r="58" spans="1:13" ht="29.1">
+      <c r="L57" s="123"/>
+      <c r="M57" s="123"/>
+    </row>
+    <row r="58" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>202</v>
       </c>
@@ -5816,10 +5838,10 @@
       <c r="I58" s="33"/>
       <c r="J58" s="34"/>
       <c r="K58" s="33"/>
-      <c r="L58" s="117"/>
-      <c r="M58" s="117"/>
-    </row>
-    <row r="59" spans="1:13" ht="30.95">
+      <c r="L58" s="123"/>
+      <c r="M58" s="123"/>
+    </row>
+    <row r="59" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>205</v>
       </c>
@@ -5844,12 +5866,12 @@
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
     </row>
-    <row r="60" spans="1:13" ht="29.1">
+    <row r="60" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>181</v>
@@ -5869,7 +5891,7 @@
       <c r="L60" s="6"/>
       <c r="M60" s="6"/>
     </row>
-    <row r="61" spans="1:13" ht="29.1">
+    <row r="61" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>208</v>
       </c>
@@ -5894,9 +5916,9 @@
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>172</v>
@@ -5919,9 +5941,9 @@
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
     </row>
-    <row r="63" spans="1:13" ht="23.45">
+    <row r="63" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>175</v>
@@ -5944,12 +5966,12 @@
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
     </row>
-    <row r="64" spans="1:13" ht="29.1">
+    <row r="64" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>18</v>
@@ -5969,12 +5991,12 @@
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
     </row>
-    <row r="65" spans="1:13" ht="43.5">
+    <row r="65" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" s="44" t="s">
         <v>252</v>
-      </c>
-      <c r="B65" s="44" t="s">
-        <v>253</v>
       </c>
       <c r="C65" s="45" t="s">
         <v>18</v>
@@ -5986,7 +6008,7 @@
         <v>18</v>
       </c>
       <c r="F65" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G65" s="109"/>
       <c r="H65" s="22"/>
@@ -5996,12 +6018,12 @@
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
     </row>
-    <row r="66" spans="1:13" ht="43.5">
+    <row r="66" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B66" s="44" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C66" s="45" t="s">
         <v>18</v>
@@ -6013,7 +6035,7 @@
         <v>18</v>
       </c>
       <c r="F66" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G66" s="109"/>
       <c r="H66" s="22"/>
@@ -6023,7 +6045,7 @@
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
     </row>
-    <row r="67" spans="1:13" ht="29.1">
+    <row r="67" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>209</v>
       </c>
@@ -6048,7 +6070,7 @@
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
     </row>
-    <row r="68" spans="1:13" ht="29.1">
+    <row r="68" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>49</v>
       </c>
@@ -6064,23 +6086,23 @@
       <c r="E68" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F68" s="7" t="s">
-        <v>255</v>
+      <c r="F68" s="127" t="s">
+        <v>321</v>
       </c>
       <c r="G68" s="53"/>
       <c r="H68" s="29"/>
       <c r="I68" s="31"/>
       <c r="J68" s="29"/>
       <c r="K68" s="28"/>
-      <c r="L68" s="119"/>
-      <c r="M68" s="119"/>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="L68" s="124"/>
+      <c r="M68" s="124"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>181</v>
@@ -6092,22 +6114,22 @@
         <v>18</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G69" s="53"/>
       <c r="H69" s="29"/>
       <c r="I69" s="31"/>
       <c r="J69" s="29"/>
       <c r="K69" s="28"/>
-      <c r="L69" s="119"/>
-      <c r="M69" s="119"/>
-    </row>
-    <row r="70" spans="1:13" ht="43.5">
+      <c r="L69" s="124"/>
+      <c r="M69" s="124"/>
+    </row>
+    <row r="70" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>181</v>
@@ -6119,17 +6141,17 @@
         <v>18</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G70" s="53"/>
       <c r="H70" s="29"/>
       <c r="I70" s="31"/>
       <c r="J70" s="29"/>
       <c r="K70" s="28"/>
-      <c r="L70" s="119"/>
-      <c r="M70" s="119"/>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="L70" s="124"/>
+      <c r="M70" s="124"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>217</v>
       </c>
@@ -6154,7 +6176,7 @@
       <c r="L71" s="6"/>
       <c r="M71" s="6"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="7"/>
       <c r="C72" s="11"/>
@@ -6169,7 +6191,7 @@
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="7"/>
       <c r="C73" s="11"/>
@@ -6181,10 +6203,10 @@
       <c r="I73" s="31"/>
       <c r="J73" s="29"/>
       <c r="K73" s="28"/>
-      <c r="L73" s="119"/>
-      <c r="M73" s="119"/>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="L73" s="124"/>
+      <c r="M73" s="124"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="7"/>
       <c r="C74" s="11"/>
@@ -6196,10 +6218,10 @@
       <c r="I74" s="31"/>
       <c r="J74" s="29"/>
       <c r="K74" s="28"/>
-      <c r="L74" s="119"/>
-      <c r="M74" s="119"/>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="L74" s="124"/>
+      <c r="M74" s="124"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F75" s="30"/>
       <c r="G75" s="28"/>
       <c r="H75" s="29"/>
@@ -6209,7 +6231,7 @@
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F76" s="27"/>
       <c r="G76" s="28"/>
       <c r="H76" s="29"/>
@@ -6219,7 +6241,7 @@
       <c r="L76" s="37"/>
       <c r="M76" s="37"/>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F77" s="27"/>
       <c r="G77" s="19"/>
       <c r="H77" s="20"/>
@@ -6229,7 +6251,7 @@
       <c r="L77" s="6"/>
       <c r="M77" s="6"/>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F78" s="27"/>
       <c r="G78" s="19"/>
       <c r="H78" s="20"/>
@@ -6239,7 +6261,7 @@
       <c r="L78" s="6"/>
       <c r="M78" s="6"/>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F79" s="30"/>
       <c r="G79" s="19"/>
       <c r="H79" s="20"/>
@@ -6249,7 +6271,7 @@
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
     </row>
-    <row r="80" spans="1:13" ht="26.1">
+    <row r="80" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F80" s="27"/>
       <c r="G80" s="26"/>
       <c r="H80" s="17"/>
@@ -6259,7 +6281,7 @@
       <c r="L80" s="6"/>
       <c r="M80" s="6"/>
     </row>
-    <row r="81" spans="6:13">
+    <row r="81" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F81" s="27"/>
       <c r="G81" s="28"/>
       <c r="H81" s="29"/>
@@ -6269,7 +6291,7 @@
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
     </row>
-    <row r="82" spans="6:13">
+    <row r="82" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F82" s="27"/>
       <c r="G82" s="28"/>
       <c r="H82" s="29"/>
@@ -6279,7 +6301,7 @@
       <c r="L82" s="6"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="6:13">
+    <row r="83" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F83" s="27"/>
       <c r="G83" s="28"/>
       <c r="H83" s="29"/>
@@ -6289,7 +6311,7 @@
       <c r="L83" s="6"/>
       <c r="M83" s="6"/>
     </row>
-    <row r="84" spans="6:13">
+    <row r="84" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F84" s="27"/>
       <c r="G84" s="28"/>
       <c r="H84" s="29"/>
@@ -6299,44 +6321,32 @@
       <c r="L84" s="6"/>
       <c r="M84" s="6"/>
     </row>
-    <row r="85" spans="6:13">
+    <row r="85" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F85" s="18"/>
     </row>
-    <row r="86" spans="6:13">
+    <row r="86" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F86" s="18"/>
     </row>
-    <row r="87" spans="6:13">
+    <row r="87" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F87" s="18"/>
     </row>
-    <row r="88" spans="6:13">
+    <row r="88" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F88" s="25"/>
     </row>
-    <row r="89" spans="6:13">
+    <row r="89" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F89" s="27"/>
     </row>
-    <row r="90" spans="6:13">
+    <row r="90" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F90" s="27"/>
     </row>
-    <row r="91" spans="6:13">
+    <row r="91" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F91" s="27"/>
     </row>
-    <row r="92" spans="6:13">
+    <row r="92" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F92" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="L52:L58"/>
-    <mergeCell ref="M52:M58"/>
-    <mergeCell ref="L68:L70"/>
-    <mergeCell ref="M68:M70"/>
-    <mergeCell ref="L73:L74"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="L49:L50"/>
-    <mergeCell ref="M49:M50"/>
     <mergeCell ref="L30:L32"/>
     <mergeCell ref="M30:M32"/>
     <mergeCell ref="L33:L42"/>
@@ -6345,6 +6355,18 @@
     <mergeCell ref="M14:M25"/>
     <mergeCell ref="L27:L28"/>
     <mergeCell ref="M27:M28"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="L49:L50"/>
+    <mergeCell ref="M49:M50"/>
+    <mergeCell ref="L52:L58"/>
+    <mergeCell ref="M52:M58"/>
+    <mergeCell ref="L68:L70"/>
+    <mergeCell ref="M68:M70"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="M73:M74"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6359,11 +6381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7BD392-D2FE-48CB-ABD4-43BFAD774472}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
@@ -6376,7 +6398,7 @@
     <col min="9" max="9" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.1">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -6387,10 +6409,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="63" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>3</v>
@@ -6405,7 +6427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>7</v>
       </c>
@@ -6430,7 +6452,7 @@
       <c r="H2" s="44"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>11</v>
       </c>
@@ -6455,7 +6477,7 @@
       <c r="H3" s="44"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9" ht="29.1">
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>13</v>
       </c>
@@ -6478,11 +6500,11 @@
         <v>9</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>17</v>
       </c>
@@ -6509,7 +6531,7 @@
       </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9" ht="29.1">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>21</v>
       </c>
@@ -6534,7 +6556,7 @@
       <c r="H6" s="44"/>
       <c r="I6" s="10"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>23</v>
       </c>
@@ -6559,7 +6581,7 @@
       <c r="H7" s="46"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="1:9" ht="29.1">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>25</v>
       </c>
@@ -6584,7 +6606,7 @@
       <c r="H8" s="46"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
         <v>27</v>
       </c>
@@ -6609,7 +6631,7 @@
       <c r="H9" s="46"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" ht="29.1">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
         <v>29</v>
       </c>
@@ -6620,7 +6642,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E10" s="45" t="s">
         <v>9</v>
@@ -6634,7 +6656,7 @@
       <c r="H10" s="44"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="57.95">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="96" t="s">
         <v>217</v>
       </c>
@@ -6661,7 +6683,7 @@
       </c>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" ht="29.1">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="43" t="s">
         <v>35</v>
       </c>
@@ -6672,7 +6694,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E12" s="45" t="s">
         <v>9</v>
@@ -6686,7 +6708,7 @@
       <c r="H12" s="44"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" ht="29.1">
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>38</v>
       </c>
@@ -6697,7 +6719,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>9</v>
@@ -6711,7 +6733,7 @@
       <c r="H13" s="46"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" ht="29.1">
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
         <v>40</v>
       </c>
@@ -6722,7 +6744,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="56" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E14" s="45" t="s">
         <v>9</v>
@@ -6736,7 +6758,7 @@
       <c r="H14" s="44"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="29.1">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>43</v>
       </c>
@@ -6747,7 +6769,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E15" s="45" t="s">
         <v>9</v>
@@ -6761,7 +6783,7 @@
       <c r="H15" s="44"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="29.1">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>45</v>
       </c>
@@ -6772,7 +6794,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>9</v>
@@ -6784,11 +6806,11 @@
         <v>9</v>
       </c>
       <c r="H16" s="44" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" ht="29.1">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>49</v>
       </c>
@@ -6799,7 +6821,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="56" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E17" s="45" t="s">
         <v>9</v>
@@ -6810,10 +6832,12 @@
       <c r="G17" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="126" t="s">
+        <v>320</v>
+      </c>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" ht="29.1">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>52</v>
       </c>
@@ -6840,7 +6864,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="30.75">
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>56</v>
       </c>
@@ -6851,12 +6875,12 @@
         <v>9</v>
       </c>
       <c r="D19" s="58" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="121" t="s">
+      <c r="F19" s="112" t="s">
         <v>58</v>
       </c>
       <c r="G19" s="11" t="s">
@@ -6867,7 +6891,7 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="29.1">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>60</v>
       </c>
@@ -6878,7 +6902,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="58" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>9</v>
@@ -6894,7 +6918,7 @@
       </c>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" ht="29.1">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>64</v>
       </c>
@@ -6905,7 +6929,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="58" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>9</v>
@@ -6919,7 +6943,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="29.1">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>68</v>
       </c>
@@ -6946,7 +6970,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="29.1">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>71</v>
       </c>
@@ -6957,7 +6981,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>9</v>
@@ -6973,7 +6997,7 @@
       </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" ht="29.1">
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>75</v>
       </c>
@@ -6984,7 +7008,7 @@
         <v>18</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E24" s="11" t="s">
         <v>18</v>
@@ -6998,7 +7022,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" ht="29.1">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>77</v>
       </c>
@@ -7009,7 +7033,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="58" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E25" s="11" t="s">
         <v>18</v>
@@ -7023,7 +7047,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" ht="29.1">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>79</v>
       </c>
@@ -7034,7 +7058,7 @@
         <v>18</v>
       </c>
       <c r="D26" s="58" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>18</v>
@@ -7048,7 +7072,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="29.1">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>81</v>
       </c>
@@ -7059,7 +7083,7 @@
         <v>18</v>
       </c>
       <c r="D27" s="58" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>18</v>
@@ -7073,7 +7097,7 @@
       <c r="H27" s="7"/>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="1:9" ht="29.1">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>83</v>
       </c>
@@ -7084,7 +7108,7 @@
         <v>18</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>18</v>
@@ -7098,7 +7122,7 @@
       <c r="H28" s="7"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:9" ht="29.1">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>85</v>
       </c>
@@ -7109,7 +7133,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="58" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>18</v>
@@ -7123,7 +7147,7 @@
       <c r="H29" s="7"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" spans="1:9" ht="72.599999999999994">
+    <row r="30" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>87</v>
       </c>
@@ -7134,7 +7158,7 @@
         <v>18</v>
       </c>
       <c r="D30" s="58" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E30" s="11" t="s">
         <v>18</v>
@@ -7146,11 +7170,11 @@
         <v>18</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="29.1">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>91</v>
       </c>
@@ -7161,7 +7185,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>18</v>
@@ -7175,7 +7199,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9" ht="30.75">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
         <v>93</v>
       </c>
@@ -7186,12 +7210,12 @@
         <v>9</v>
       </c>
       <c r="D32" s="56" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E32" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="F32" s="120" t="s">
+      <c r="F32" s="117" t="s">
         <v>58</v>
       </c>
       <c r="G32" s="45" t="s">
@@ -7202,7 +7226,7 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:9" ht="29.1">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
         <v>95</v>
       </c>
@@ -7213,7 +7237,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="56" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E33" s="45" t="s">
         <v>9</v>
@@ -7229,7 +7253,7 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="1:9" ht="29.1">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
         <v>98</v>
       </c>
@@ -7240,7 +7264,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="56" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E34" s="45" t="s">
         <v>9</v>
@@ -7254,7 +7278,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="1:9" ht="29.1">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
         <v>100</v>
       </c>
@@ -7281,18 +7305,18 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="1:9" ht="29.1">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C36" s="47" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="56" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E36" s="47" t="s">
         <v>18</v>
@@ -7306,7 +7330,7 @@
       <c r="H36" s="44"/>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="1:9" ht="29.1">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>103</v>
       </c>
@@ -7317,7 +7341,7 @@
         <v>18</v>
       </c>
       <c r="D37" s="56" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E37" s="47" t="s">
         <v>18</v>
@@ -7331,7 +7355,7 @@
       <c r="H37" s="44"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="1:9" ht="29.1">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
         <v>105</v>
       </c>
@@ -7342,7 +7366,7 @@
         <v>18</v>
       </c>
       <c r="D38" s="56" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E38" s="47" t="s">
         <v>18</v>
@@ -7356,7 +7380,7 @@
       <c r="H38" s="44"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="1:9" ht="29.1">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>107</v>
       </c>
@@ -7367,7 +7391,7 @@
         <v>18</v>
       </c>
       <c r="D39" s="56" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E39" s="47" t="s">
         <v>18</v>
@@ -7381,7 +7405,7 @@
       <c r="H39" s="44"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" ht="29.1">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>109</v>
       </c>
@@ -7392,7 +7416,7 @@
         <v>18</v>
       </c>
       <c r="D40" s="56" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E40" s="47" t="s">
         <v>18</v>
@@ -7406,7 +7430,7 @@
       <c r="H40" s="46"/>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="1:9" ht="29.1">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>111</v>
       </c>
@@ -7417,7 +7441,7 @@
         <v>18</v>
       </c>
       <c r="D41" s="56" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E41" s="47" t="s">
         <v>18</v>
@@ -7431,7 +7455,7 @@
       <c r="H41" s="44"/>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="1:9" ht="29.1">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
         <v>113</v>
       </c>
@@ -7442,7 +7466,7 @@
         <v>18</v>
       </c>
       <c r="D42" s="56" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E42" s="47" t="s">
         <v>18</v>
@@ -7456,7 +7480,7 @@
       <c r="H42" s="44"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:9" ht="29.1">
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>115</v>
       </c>
@@ -7467,7 +7491,7 @@
         <v>117</v>
       </c>
       <c r="D43" s="58" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E43" s="11" t="s">
         <v>117</v>
@@ -7483,7 +7507,7 @@
       </c>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:9" ht="57.95">
+    <row r="44" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>120</v>
       </c>
@@ -7494,7 +7518,7 @@
         <v>117</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E44" s="11" t="s">
         <v>117</v>
@@ -7506,11 +7530,11 @@
         <v>117</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="1:9" ht="29.1">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>124</v>
       </c>
@@ -7521,7 +7545,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E45" s="11" t="s">
         <v>9</v>
@@ -7535,7 +7559,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:9" ht="29.1">
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>127</v>
       </c>
@@ -7546,7 +7570,7 @@
         <v>18</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E46" s="11" t="s">
         <v>18</v>
@@ -7560,7 +7584,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="1:9" ht="29.1">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>130</v>
       </c>
@@ -7585,7 +7609,7 @@
       <c r="H47" s="7"/>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="1:9" ht="29.1">
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>133</v>
       </c>
@@ -7610,7 +7634,7 @@
       <c r="H48" s="7"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="1:9" ht="29.1">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>135</v>
       </c>
@@ -7635,7 +7659,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="10"/>
     </row>
-    <row r="50" spans="1:9" ht="29.1">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>138</v>
       </c>
@@ -7660,7 +7684,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="1:9" ht="29.1">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>141</v>
       </c>
@@ -7685,7 +7709,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="1:9" ht="29.1">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>18</v>
       </c>
@@ -7696,50 +7720,50 @@
         <v>18</v>
       </c>
       <c r="D52" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E52" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="E52" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H52" s="10" t="s">
+      <c r="E53" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="E53" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>305</v>
-      </c>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="1:9" ht="43.5">
+    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="43" t="s">
         <v>143</v>
       </c>
@@ -7766,7 +7790,7 @@
       </c>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="1:9" ht="29.1">
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="104" t="s">
         <v>147</v>
       </c>
@@ -7793,7 +7817,7 @@
       </c>
       <c r="I55" s="10"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>150</v>
       </c>
@@ -7820,7 +7844,7 @@
       </c>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>153</v>
       </c>
@@ -7847,7 +7871,7 @@
       </c>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="1:9" ht="91.5">
+    <row r="58" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>156</v>
       </c>
@@ -7869,12 +7893,12 @@
       <c r="G58" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H58" s="124" t="s">
+      <c r="H58" s="127" t="s">
         <v>159</v>
       </c>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="1:9" ht="29.1">
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>160</v>
       </c>
@@ -7901,7 +7925,7 @@
       </c>
       <c r="I59" s="10"/>
     </row>
-    <row r="60" spans="1:9" ht="87">
+    <row r="60" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>164</v>
       </c>
@@ -7924,11 +7948,11 @@
         <v>9</v>
       </c>
       <c r="H60" s="112" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="I60" s="112"/>
     </row>
-    <row r="61" spans="1:9" ht="391.5">
+    <row r="61" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>168</v>
       </c>
@@ -7947,9 +7971,9 @@
       </c>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" spans="1:9" ht="409.5">
+    <row r="62" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B62" s="108" t="s">
         <v>18</v>
@@ -7970,11 +7994,11 @@
         <v>9</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I62" s="10"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>171</v>
       </c>
@@ -8001,7 +8025,7 @@
       </c>
       <c r="I63" s="10"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>174</v>
       </c>
@@ -8028,7 +8052,7 @@
       </c>
       <c r="I64" s="10"/>
     </row>
-    <row r="65" spans="1:9" ht="29.1">
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
         <v>179</v>
       </c>
@@ -8039,7 +8063,7 @@
         <v>181</v>
       </c>
       <c r="D65" s="44" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E65" s="49" t="s">
         <v>9</v>
@@ -8053,7 +8077,7 @@
       <c r="H65" s="44"/>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="1:9" ht="29.1">
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
         <v>183</v>
       </c>
@@ -8064,7 +8088,7 @@
         <v>181</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E66" s="49" t="s">
         <v>9</v>
@@ -8078,7 +8102,7 @@
       <c r="H66" s="44"/>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" spans="1:9" ht="29.1">
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="43" t="s">
         <v>186</v>
       </c>
@@ -8089,7 +8113,7 @@
         <v>181</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E67" s="49" t="s">
         <v>9</v>
@@ -8103,18 +8127,18 @@
       <c r="H67" s="44"/>
       <c r="I67" s="10"/>
     </row>
-    <row r="68" spans="1:9" ht="29.1">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="43" t="s">
         <v>189</v>
       </c>
       <c r="B68" s="44" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C68" s="49" t="s">
         <v>181</v>
       </c>
       <c r="D68" s="44" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E68" s="49" t="s">
         <v>9</v>
@@ -8128,7 +8152,7 @@
       <c r="H68" s="44"/>
       <c r="I68" s="10"/>
     </row>
-    <row r="69" spans="1:9" ht="29.1">
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="43" t="s">
         <v>191</v>
       </c>
@@ -8139,7 +8163,7 @@
         <v>18</v>
       </c>
       <c r="D69" s="57" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E69" s="47" t="s">
         <v>18</v>
@@ -8153,7 +8177,7 @@
       <c r="H69" s="46"/>
       <c r="I69" s="10"/>
     </row>
-    <row r="70" spans="1:9" ht="29.1">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="43" t="s">
         <v>194</v>
       </c>
@@ -8178,7 +8202,7 @@
       <c r="H70" s="46"/>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="1:9" ht="29.1">
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>198</v>
       </c>
@@ -8203,7 +8227,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="1:9" ht="29.1">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>198</v>
       </c>
@@ -8228,7 +8252,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="10"/>
     </row>
-    <row r="73" spans="1:9" ht="29.1">
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>202</v>
       </c>
@@ -8255,7 +8279,7 @@
       </c>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9" ht="29.1">
+    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>205</v>
       </c>
@@ -8282,7 +8306,7 @@
       </c>
       <c r="I74" s="10"/>
     </row>
-    <row r="75" spans="1:9" ht="29.1">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>208</v>
       </c>
@@ -8307,7 +8331,7 @@
       <c r="H75" s="7"/>
       <c r="I75" s="10"/>
     </row>
-    <row r="76" spans="1:9" ht="29.1">
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="43" t="s">
         <v>209</v>
       </c>
@@ -8332,7 +8356,7 @@
       <c r="H76" s="44"/>
       <c r="I76" s="10"/>
     </row>
-    <row r="77" spans="1:9" ht="57.95">
+    <row r="77" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>217</v>
       </c>
@@ -8372,11 +8396,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018E8C56-7845-49A6-99BD-BE444F662575}">
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="37.42578125" style="78" customWidth="1"/>
@@ -8389,7 +8413,7 @@
     <col min="9" max="9" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.1">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -8406,10 +8430,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>5</v>
@@ -8418,7 +8442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>7</v>
       </c>
@@ -8443,7 +8467,7 @@
       <c r="H2" s="44"/>
       <c r="I2" s="109"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>11</v>
       </c>
@@ -8468,7 +8492,7 @@
       <c r="H3" s="44"/>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>17</v>
       </c>
@@ -8493,7 +8517,7 @@
       </c>
       <c r="I4" s="109"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
         <v>13</v>
       </c>
@@ -8518,7 +8542,7 @@
       <c r="H5" s="44"/>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>35</v>
       </c>
@@ -8535,7 +8559,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="75" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G6" s="67" t="s">
         <v>9</v>
@@ -8545,7 +8569,7 @@
       </c>
       <c r="I6" s="109"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="s">
         <v>38</v>
       </c>
@@ -8562,7 +8586,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="68" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G7" s="67" t="s">
         <v>9</v>
@@ -8572,7 +8596,7 @@
       </c>
       <c r="I7" s="109"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
         <v>21</v>
       </c>
@@ -8599,7 +8623,7 @@
       </c>
       <c r="I8" s="109"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -8616,7 +8640,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G9" s="71" t="s">
         <v>9</v>
@@ -8624,7 +8648,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>215</v>
       </c>
@@ -8641,7 +8665,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="70" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G10" s="71" t="s">
         <v>9</v>
@@ -8651,7 +8675,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
@@ -8676,7 +8700,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
@@ -8701,7 +8725,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>27</v>
       </c>
@@ -8726,12 +8750,12 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="93" t="s">
         <v>217</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" s="99" t="s">
         <v>9</v>
@@ -8751,11 +8775,11 @@
       <c r="H14" s="95"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" ht="30.75">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="118" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="45" t="s">
@@ -8768,7 +8792,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G15" s="67" t="s">
         <v>9</v>
@@ -8776,7 +8800,7 @@
       <c r="H15" s="44"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" ht="29.1">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="43" t="s">
         <v>68</v>
       </c>
@@ -8801,7 +8825,7 @@
       <c r="H16" s="44"/>
       <c r="I16" s="109"/>
     </row>
-    <row r="17" spans="1:9" ht="29.1">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>71</v>
       </c>
@@ -8818,7 +8842,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="68" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G17" s="67" t="s">
         <v>9</v>
@@ -8826,7 +8850,7 @@
       <c r="H17" s="44"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" ht="29.1">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>60</v>
       </c>
@@ -8843,7 +8867,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="68" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G18" s="67" t="s">
         <v>9</v>
@@ -8851,7 +8875,7 @@
       <c r="H18" s="107"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>64</v>
       </c>
@@ -8868,7 +8892,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="68" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G19" s="67" t="s">
         <v>9</v>
@@ -8878,11 +8902,11 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" ht="30.75">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="123" t="s">
+      <c r="B20" s="119" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -8895,7 +8919,7 @@
         <v>9</v>
       </c>
       <c r="F20" s="70" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G20" s="71" t="s">
         <v>9</v>
@@ -8903,7 +8927,7 @@
       <c r="H20" s="7"/>
       <c r="I20" s="109"/>
     </row>
-    <row r="21" spans="1:9" ht="29.1">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>100</v>
       </c>
@@ -8928,7 +8952,7 @@
       <c r="H21" s="7"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" ht="29.1">
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>101</v>
       </c>
@@ -8939,13 +8963,13 @@
         <v>18</v>
       </c>
       <c r="D22" s="63" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G22" s="71" t="s">
         <v>18</v>
@@ -8953,7 +8977,7 @@
       <c r="H22" s="7"/>
       <c r="I22" s="109"/>
     </row>
-    <row r="23" spans="1:9" ht="43.5">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>95</v>
       </c>
@@ -8970,7 +8994,7 @@
         <v>9</v>
       </c>
       <c r="F23" s="70" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G23" s="71" t="s">
         <v>9</v>
@@ -8980,7 +9004,7 @@
       </c>
       <c r="I23" s="109"/>
     </row>
-    <row r="24" spans="1:9" ht="101.45">
+    <row r="24" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>98</v>
       </c>
@@ -8997,7 +9021,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="70" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G24" s="71" t="s">
         <v>9</v>
@@ -9007,7 +9031,7 @@
       </c>
       <c r="I24" s="109"/>
     </row>
-    <row r="25" spans="1:9" ht="29.1">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="43" t="s">
         <v>115</v>
       </c>
@@ -9024,7 +9048,7 @@
         <v>117</v>
       </c>
       <c r="F25" s="68" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G25" s="45" t="s">
         <v>117</v>
@@ -9034,12 +9058,12 @@
       </c>
       <c r="I25" s="109"/>
     </row>
-    <row r="26" spans="1:9" ht="43.5">
+    <row r="26" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="B26" s="80" t="s">
-        <v>223</v>
+      <c r="B26" s="128" t="s">
+        <v>322</v>
       </c>
       <c r="C26" s="45" t="s">
         <v>117</v>
@@ -9051,17 +9075,17 @@
         <v>117</v>
       </c>
       <c r="F26" s="68" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G26" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="H26" s="44" t="s">
-        <v>119</v>
+      <c r="H26" s="126" t="s">
+        <v>323</v>
       </c>
       <c r="I26" s="109"/>
     </row>
-    <row r="27" spans="1:9" ht="29.1">
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
         <v>124</v>
       </c>
@@ -9078,7 +9102,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="75" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="G27" s="67" t="s">
         <v>9</v>
@@ -9086,7 +9110,7 @@
       <c r="H27" s="44"/>
       <c r="I27" s="109"/>
     </row>
-    <row r="28" spans="1:9" ht="29.1">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>127</v>
       </c>
@@ -9103,7 +9127,7 @@
         <v>18</v>
       </c>
       <c r="F28" s="75" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G28" s="67" t="s">
         <v>18</v>
@@ -9111,7 +9135,7 @@
       <c r="H28" s="44"/>
       <c r="I28" s="109"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>130</v>
       </c>
@@ -9136,7 +9160,7 @@
       <c r="H29" s="44"/>
       <c r="I29" s="109"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
         <v>135</v>
       </c>
@@ -9161,7 +9185,7 @@
       <c r="H30" s="44"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" ht="29.1">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
         <v>138</v>
       </c>
@@ -9186,39 +9210,39 @@
       <c r="H31" s="44"/>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="77" t="s">
         <v>224</v>
       </c>
-      <c r="B32" s="77" t="s">
+      <c r="C32" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="C32" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="77" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="46" t="s">
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="43" t="s">
+      <c r="B33" s="77" t="s">
         <v>227</v>
-      </c>
-      <c r="B33" s="77" t="s">
-        <v>228</v>
       </c>
       <c r="C33" s="47" t="s">
         <v>18</v>
@@ -9238,12 +9262,12 @@
       <c r="H33" s="46"/>
       <c r="I33" s="109"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B34" s="77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" s="45" t="s">
         <v>18</v>
@@ -9263,7 +9287,7 @@
       <c r="H34" s="44"/>
       <c r="I34" s="109"/>
     </row>
-    <row r="35" spans="1:9" ht="29.1">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>52</v>
       </c>
@@ -9290,12 +9314,12 @@
       </c>
       <c r="I35" s="109"/>
     </row>
-    <row r="36" spans="1:9" ht="29.1">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>143</v>
       </c>
       <c r="B36" s="82" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>18</v>
@@ -9317,7 +9341,7 @@
       </c>
       <c r="I36" s="109"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="101" t="s">
         <v>147</v>
       </c>
@@ -9342,7 +9366,7 @@
       <c r="H37" s="103"/>
       <c r="I37" s="109"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="43" t="s">
         <v>150</v>
       </c>
@@ -9365,11 +9389,11 @@
         <v>18</v>
       </c>
       <c r="H38" s="46" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I38" s="109"/>
     </row>
-    <row r="39" spans="1:9" ht="57.95">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="43" t="s">
         <v>153</v>
       </c>
@@ -9392,11 +9416,11 @@
         <v>18</v>
       </c>
       <c r="H39" s="46" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I39" s="109"/>
     </row>
-    <row r="40" spans="1:9" ht="29.1">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="43" t="s">
         <v>156</v>
       </c>
@@ -9419,11 +9443,11 @@
         <v>18</v>
       </c>
       <c r="H40" s="44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I40" s="109"/>
     </row>
-    <row r="41" spans="1:9" ht="29.1">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="43" t="s">
         <v>160</v>
       </c>
@@ -9448,7 +9472,7 @@
       <c r="H41" s="43"/>
       <c r="I41" s="109"/>
     </row>
-    <row r="42" spans="1:9" ht="72.599999999999994">
+    <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>164</v>
       </c>
@@ -9471,16 +9495,16 @@
         <v>18</v>
       </c>
       <c r="H42" s="112" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="1:9" ht="29.1">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>9</v>
@@ -9492,7 +9516,7 @@
         <v>9</v>
       </c>
       <c r="F43" s="70" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G43" s="71" t="s">
         <v>9</v>
@@ -9500,12 +9524,12 @@
       <c r="H43" s="7"/>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="1:9" ht="29.1">
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>9</v>
@@ -9517,7 +9541,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="70" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G44" s="71" t="s">
         <v>9</v>
@@ -9525,7 +9549,7 @@
       <c r="H44" s="7"/>
       <c r="I44" s="112"/>
     </row>
-    <row r="45" spans="1:9" ht="29.1">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>171</v>
       </c>
@@ -9548,11 +9572,11 @@
         <v>18</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="1:9" ht="29.1">
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>174</v>
       </c>
@@ -9575,16 +9599,16 @@
         <v>18</v>
       </c>
       <c r="H46" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I46" s="109"/>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="I46" s="109"/>
-    </row>
-    <row r="47" spans="1:9" ht="29.1">
-      <c r="A47" s="9" t="s">
+      <c r="B47" s="63" t="s">
         <v>236</v>
-      </c>
-      <c r="B47" s="63" t="s">
-        <v>237</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>9</v>
@@ -9596,7 +9620,7 @@
         <v>18</v>
       </c>
       <c r="F47" s="73" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G47" s="42" t="s">
         <v>18</v>
@@ -9604,7 +9628,7 @@
       <c r="H47" s="10"/>
       <c r="I47" s="109"/>
     </row>
-    <row r="48" spans="1:9" ht="43.5">
+    <row r="48" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="43" t="s">
         <v>179</v>
       </c>
@@ -9621,17 +9645,17 @@
         <v>181</v>
       </c>
       <c r="F48" s="75" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G48" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="126" t="s">
-        <v>319</v>
+      <c r="H48" s="122" t="s">
+        <v>317</v>
       </c>
       <c r="I48" s="109"/>
     </row>
-    <row r="49" spans="1:9" ht="29.1">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="43" t="s">
         <v>183</v>
       </c>
@@ -9648,7 +9672,7 @@
         <v>181</v>
       </c>
       <c r="F49" s="75" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G49" s="69" t="s">
         <v>9</v>
@@ -9656,7 +9680,7 @@
       <c r="H49" s="44"/>
       <c r="I49" s="109"/>
     </row>
-    <row r="50" spans="1:9" ht="29.1">
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="43" t="s">
         <v>186</v>
       </c>
@@ -9673,17 +9697,17 @@
         <v>181</v>
       </c>
       <c r="F50" s="75" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G50" s="69" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="44" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I50" s="109"/>
     </row>
-    <row r="51" spans="1:9" ht="29.1">
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="43" t="s">
         <v>191</v>
       </c>
@@ -9700,17 +9724,17 @@
         <v>181</v>
       </c>
       <c r="F51" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="G51" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="G51" s="69" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="44" t="s">
-        <v>240</v>
-      </c>
       <c r="I51" s="109"/>
     </row>
-    <row r="52" spans="1:9" ht="29.1">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="43" t="s">
         <v>194</v>
       </c>
@@ -9735,9 +9759,9 @@
       <c r="H52" s="44"/>
       <c r="I52" s="109"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B53" s="80" t="s">
         <v>172</v>
@@ -9760,9 +9784,9 @@
       <c r="H53" s="44"/>
       <c r="I53" s="109"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B54" s="80" t="s">
         <v>175</v>
@@ -9785,12 +9809,12 @@
       <c r="H54" s="44"/>
       <c r="I54" s="109"/>
     </row>
-    <row r="55" spans="1:9" ht="29.1">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="43" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" s="80" t="s">
         <v>243</v>
-      </c>
-      <c r="B55" s="80" t="s">
-        <v>244</v>
       </c>
       <c r="C55" s="45" t="s">
         <v>18</v>
@@ -9810,12 +9834,12 @@
       <c r="H55" s="46"/>
       <c r="I55" s="109"/>
     </row>
-    <row r="56" spans="1:9" ht="29.1">
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B56" s="80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C56" s="45" t="s">
         <v>18</v>
@@ -9835,7 +9859,7 @@
       <c r="H56" s="44"/>
       <c r="I56" s="109"/>
     </row>
-    <row r="57" spans="1:9" ht="29.1">
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="43" t="s">
         <v>189</v>
       </c>
@@ -9852,17 +9876,17 @@
         <v>181</v>
       </c>
       <c r="F57" s="75" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G57" s="69" t="s">
         <v>9</v>
       </c>
       <c r="H57" s="44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="1:9" ht="29.1">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>202</v>
       </c>
@@ -9887,7 +9911,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="1:9" ht="29.1">
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>205</v>
       </c>
@@ -9912,12 +9936,12 @@
       <c r="H59" s="7"/>
       <c r="I59" s="10"/>
     </row>
-    <row r="60" spans="1:9" ht="29.1">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="B60" s="81" t="s">
         <v>247</v>
-      </c>
-      <c r="B60" s="81" t="s">
-        <v>248</v>
       </c>
       <c r="C60" s="42" t="s">
         <v>181</v>
@@ -9937,7 +9961,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="1:9" ht="29.1">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>208</v>
       </c>
@@ -9962,9 +9986,9 @@
       <c r="H61" s="7"/>
       <c r="I61" s="109"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B62" s="63" t="s">
         <v>172</v>
@@ -9987,9 +10011,9 @@
       <c r="H62" s="7"/>
       <c r="I62" s="111"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B63" s="63" t="s">
         <v>175</v>
@@ -10012,12 +10036,12 @@
       <c r="H63" s="7"/>
       <c r="I63" s="111"/>
     </row>
-    <row r="64" spans="1:9" ht="29.1">
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B64" s="63" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>18</v>
@@ -10037,12 +10061,12 @@
       <c r="H64" s="10"/>
       <c r="I64" s="111"/>
     </row>
-    <row r="65" spans="1:9" ht="57.95">
+    <row r="65" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" s="80" t="s">
         <v>252</v>
-      </c>
-      <c r="B65" s="80" t="s">
-        <v>253</v>
       </c>
       <c r="C65" s="45" t="s">
         <v>18</v>
@@ -10060,22 +10084,22 @@
         <v>18</v>
       </c>
       <c r="H65" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I65" s="109"/>
     </row>
-    <row r="66" spans="1:9" ht="57.95">
+    <row r="66" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="43" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B66" s="80" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C66" s="45" t="s">
         <v>18</v>
       </c>
       <c r="D66" s="77" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E66" s="47" t="s">
         <v>18</v>
@@ -10087,11 +10111,11 @@
         <v>18</v>
       </c>
       <c r="H66" s="44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I66" s="109"/>
     </row>
-    <row r="67" spans="1:9" ht="29.1">
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>209</v>
       </c>
@@ -10116,7 +10140,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="109"/>
     </row>
-    <row r="68" spans="1:9" ht="29.1">
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>49</v>
       </c>
@@ -10133,22 +10157,22 @@
         <v>9</v>
       </c>
       <c r="F68" s="70" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G68" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="H68" s="7" t="s">
-        <v>322</v>
+      <c r="H68" s="127" t="s">
+        <v>321</v>
       </c>
       <c r="I68" s="109"/>
     </row>
-    <row r="69" spans="1:9" ht="29.1">
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B69" s="63" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>181</v>
@@ -10166,16 +10190,16 @@
         <v>18</v>
       </c>
       <c r="H69" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B70" s="63" t="s">
         <v>258</v>
-      </c>
-      <c r="I69" s="10"/>
-    </row>
-    <row r="70" spans="1:9" ht="43.5">
-      <c r="A70" s="9" t="s">
-        <v>259</v>
-      </c>
-      <c r="B70" s="63" t="s">
-        <v>260</v>
       </c>
       <c r="C70" s="11" t="s">
         <v>181</v>
@@ -10193,11 +10217,11 @@
         <v>18</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="63"/>
       <c r="C71" s="11"/>
@@ -10208,7 +10232,7 @@
       <c r="H71" s="7"/>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="63"/>
       <c r="C72" s="11"/>
@@ -10219,7 +10243,7 @@
       <c r="H72" s="7"/>
       <c r="I72" s="10"/>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="63"/>
       <c r="C73" s="11"/>
@@ -10230,7 +10254,7 @@
       <c r="H73" s="7"/>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="63"/>
       <c r="C74" s="11"/>
@@ -10251,6 +10275,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100CE3A8153F207434E9AE9E016B63FAED4" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="52bf93efd82d4e5a4b2dd25d42b7cc87">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee8ef5dc-6422-4132-ba28-a9150fefde4c" xmlns:ns3="672a50b0-1df9-4341-9d54-48b9c706e195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02e2b7d272b82d896a959b2d413e6733" ns2:_="" ns3:_="">
     <xsd:import namespace="ee8ef5dc-6422-4132-ba28-a9150fefde4c"/>
@@ -10479,15 +10512,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10500,13 +10524,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4853F2AD-502C-4C24-9E91-19FB43DFD771}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912B5AAF-FD1D-4092-AB11-BCD9ECA30C35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{912B5AAF-FD1D-4092-AB11-BCD9ECA30C35}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4853F2AD-502C-4C24-9E91-19FB43DFD771}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee8ef5dc-6422-4132-ba28-a9150fefde4c"/>
+    <ds:schemaRef ds:uri="672a50b0-1df9-4341-9d54-48b9c706e195"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E44D686-25A5-46EE-BE4F-34D7EEAF48C5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E44D686-25A5-46EE-BE4F-34D7EEAF48C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee8ef5dc-6422-4132-ba28-a9150fefde4c"/>
+    <ds:schemaRef ds:uri="672a50b0-1df9-4341-9d54-48b9c706e195"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>